<commit_message>
herschrijven feature in onderzoek (nog in bewerking)
rules voor afgeleide gegevens
</commit_message>
<xml_diff>
--- a/features/in onderzoek.xlsx
+++ b/features/in onderzoek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/GitHub/Haal-Centraal-BRP-bevragen/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214AF458-B826-944B-B2FE-D840D8786B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52857A13-2D74-864D-9792-9542DF167565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 persoon" sheetId="4" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="271">
   <si>
     <t>API</t>
   </si>
@@ -773,12 +773,6 @@
     <t>Reisdocument</t>
   </si>
   <si>
-    <t>identificatiecodeVerblijfplaats</t>
-  </si>
-  <si>
-    <t>woonplaatsnaam</t>
-  </si>
-  <si>
     <t>huisnummertoevoeging</t>
   </si>
   <si>
@@ -981,9 +975,6 @@
   </si>
   <si>
     <t>090330</t>
-  </si>
-  <si>
-    <t>adellijkeTitelPredikaat</t>
   </si>
   <si>
     <t>voorletters</t>
@@ -1066,6 +1057,18 @@
   </si>
   <si>
     <t>adresregel3</t>
+  </si>
+  <si>
+    <t>woonplaats</t>
+  </si>
+  <si>
+    <t>adresseerbaarObjectIdentificatie</t>
+  </si>
+  <si>
+    <t>nummeraanduidingIdentificatie</t>
+  </si>
+  <si>
+    <t>adellijkeTitelPredicaat</t>
   </si>
 </sst>
 </file>
@@ -1799,9 +1802,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1821,7 +1824,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>77</v>
@@ -1829,7 +1832,7 @@
     </row>
     <row r="2" spans="1:17" s="9" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>3</v>
@@ -1838,13 +1841,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="G2" s="36" t="s">
         <v>21</v>
@@ -1853,22 +1856,22 @@
         <v>22</v>
       </c>
       <c r="I2" s="48" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J2" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="M2" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="N2" s="48" t="s">
         <v>244</v>
-      </c>
-      <c r="L2" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="M2" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="N2" s="48" t="s">
-        <v>247</v>
       </c>
       <c r="O2" s="35" t="s">
         <v>29</v>
@@ -2198,7 +2201,7 @@
     </row>
     <row r="17" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B17" s="15"/>
       <c r="E17" s="26"/>
@@ -2221,7 +2224,7 @@
     </row>
     <row r="18" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B18" s="19"/>
       <c r="E18" s="19"/>
@@ -2892,7 +2895,7 @@
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" ht="133" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>46</v>
@@ -3387,10 +3390,10 @@
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="J2" s="34"/>
       <c r="K2" s="34"/>
@@ -5117,7 +5120,7 @@
   <dimension ref="A1:M204"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5138,7 +5141,7 @@
         <v>145</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>77</v>
@@ -5146,7 +5149,7 @@
     </row>
     <row r="2" spans="1:13" s="53" customFormat="1" ht="200" x14ac:dyDescent="0.2">
       <c r="A2" s="62" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>3</v>
@@ -5155,13 +5158,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E2" s="51" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>21</v>
@@ -5170,7 +5173,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="52" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J2" s="51" t="s">
         <v>29</v>
@@ -5255,7 +5258,7 @@
     </row>
     <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="21"/>
@@ -5282,7 +5285,7 @@
     </row>
     <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="21"/>
@@ -5298,7 +5301,7 @@
     </row>
     <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="21"/>
@@ -5312,7 +5315,7 @@
     </row>
     <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="21"/>
@@ -5326,7 +5329,7 @@
     </row>
     <row r="10" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="21"/>
@@ -5343,7 +5346,7 @@
     </row>
     <row r="11" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B11" s="30"/>
       <c r="E11" s="15"/>
@@ -5364,7 +5367,7 @@
     </row>
     <row r="12" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B12" s="30"/>
       <c r="E12" s="19"/>
@@ -5379,7 +5382,7 @@
     </row>
     <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B13" s="30"/>
       <c r="E13" s="19"/>
@@ -5394,7 +5397,7 @@
     </row>
     <row r="14" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B14" s="30"/>
       <c r="E14" s="19"/>
@@ -5435,7 +5438,7 @@
     </row>
     <row r="17" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="33"/>
@@ -5448,7 +5451,7 @@
     </row>
     <row r="18" spans="1:13" s="46" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B18" s="45"/>
       <c r="D18" s="47" t="s">
@@ -5526,7 +5529,7 @@
     </row>
     <row r="22" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="21"/>
@@ -5551,7 +5554,7 @@
     </row>
     <row r="23" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="21"/>
@@ -5569,7 +5572,7 @@
     </row>
     <row r="24" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="21"/>
@@ -5585,7 +5588,7 @@
     </row>
     <row r="25" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="21"/>
@@ -5599,7 +5602,7 @@
     </row>
     <row r="26" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="21"/>
@@ -5616,7 +5619,7 @@
     </row>
     <row r="27" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B27" s="30"/>
       <c r="E27" s="15"/>
@@ -5637,7 +5640,7 @@
     </row>
     <row r="28" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B28" s="30"/>
       <c r="E28" s="19"/>
@@ -5652,7 +5655,7 @@
     </row>
     <row r="29" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B29" s="30"/>
       <c r="E29" s="19"/>
@@ -5667,7 +5670,7 @@
     </row>
     <row r="30" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B30" s="30"/>
       <c r="E30" s="19"/>
@@ -5710,7 +5713,7 @@
     </row>
     <row r="33" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="33"/>
@@ -5729,7 +5732,7 @@
     </row>
     <row r="34" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="21"/>
@@ -7244,7 +7247,7 @@
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>24</v>
@@ -7253,7 +7256,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -7751,7 +7754,7 @@
   <dimension ref="A1:R191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7775,21 +7778,21 @@
         <v>141</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>77</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="53" customFormat="1" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>3</v>
@@ -7804,7 +7807,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="G2" s="52" t="s">
         <v>21</v>
@@ -7813,7 +7816,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="52" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J2" s="51" t="s">
         <v>29</v>
@@ -7834,13 +7837,13 @@
         <v>31</v>
       </c>
       <c r="P2" s="51" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="Q2" s="52" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R2" s="52" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -7890,13 +7893,13 @@
         <v>79</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -7933,7 +7936,7 @@
     </row>
     <row r="6" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B6" s="30"/>
       <c r="E6" s="15" t="s">
@@ -7956,18 +7959,18 @@
       <c r="L6" s="16"/>
       <c r="M6" s="19"/>
       <c r="P6" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B7" s="30"/>
       <c r="E7" s="19" t="s">
@@ -7982,7 +7985,7 @@
     </row>
     <row r="8" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B8" s="30"/>
       <c r="E8" s="19"/>
@@ -7992,18 +7995,18 @@
       <c r="J8" s="19"/>
       <c r="M8" s="19"/>
       <c r="P8" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B9" s="30"/>
       <c r="E9" s="19"/>
@@ -8013,18 +8016,18 @@
       <c r="J9" s="19"/>
       <c r="M9" s="19"/>
       <c r="P9" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B10" s="30"/>
       <c r="E10" s="19"/>
@@ -8037,18 +8040,18 @@
       <c r="L10" s="31"/>
       <c r="M10" s="19"/>
       <c r="P10" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" s="30"/>
       <c r="E11" s="15"/>
@@ -8072,7 +8075,7 @@
     </row>
     <row r="12" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B12" s="30"/>
       <c r="E12" s="19"/>
@@ -8088,7 +8091,7 @@
     </row>
     <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B13" s="30"/>
       <c r="E13" s="19"/>
@@ -8104,7 +8107,7 @@
     </row>
     <row r="14" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B14" s="30"/>
       <c r="E14" s="19"/>
@@ -8150,7 +8153,7 @@
     </row>
     <row r="17" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B17" s="19"/>
       <c r="D17" s="31"/>
@@ -8171,7 +8174,7 @@
     </row>
     <row r="18" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B18" s="19"/>
       <c r="D18" s="31"/>
@@ -8188,7 +8191,7 @@
     </row>
     <row r="19" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B19" s="19"/>
       <c r="D19" s="31"/>
@@ -8205,7 +8208,7 @@
     </row>
     <row r="20" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B20" s="19"/>
       <c r="D20" s="31"/>
@@ -10112,7 +10115,7 @@
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" ht="93" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>29</v>
@@ -10124,7 +10127,7 @@
         <v>31</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F2" s="63"/>
     </row>
@@ -10722,9 +10725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456F4B46-E245-DB4D-BC75-1E1265C64598}">
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R21" sqref="R21"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10742,12 +10745,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="9" customFormat="1" ht="178" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="171" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C2" s="38" t="s">
         <v>39</v>
@@ -10759,34 +10762,34 @@
         <v>52</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I2" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>178</v>
-      </c>
       <c r="L2" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>173</v>
+        <v>267</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>172</v>
+        <v>268</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>35</v>
+        <v>269</v>
       </c>
       <c r="P2" s="37" t="s">
         <v>36</v>
@@ -10795,13 +10798,13 @@
         <v>31</v>
       </c>
       <c r="R2" s="37" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="S2" s="37" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="T2" s="37" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="U2" s="37" t="s">
         <v>41</v>
@@ -10813,13 +10816,13 @@
         <v>42</v>
       </c>
       <c r="X2" s="38" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Y2" s="38" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="Z2" s="38" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -10913,6 +10916,9 @@
         <v>79</v>
       </c>
       <c r="D4" s="17"/>
+      <c r="M4" s="16" t="s">
+        <v>79</v>
+      </c>
       <c r="S4" s="16" t="s">
         <v>79</v>
       </c>
@@ -10920,13 +10926,16 @@
     </row>
     <row r="5" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="21"/>
+      <c r="M5" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="W5" s="21"/>
     </row>
     <row r="6" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -11024,7 +11033,7 @@
     </row>
     <row r="11" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="43"/>
@@ -11042,7 +11051,7 @@
     </row>
     <row r="12" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B12" s="41"/>
       <c r="C12" s="43"/>
@@ -11057,7 +11066,7 @@
     </row>
     <row r="13" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B13" s="41"/>
       <c r="C13" s="43"/>
@@ -11072,7 +11081,7 @@
     </row>
     <row r="14" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="43"/>
@@ -11087,7 +11096,7 @@
     </row>
     <row r="15" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B15" s="41"/>
       <c r="C15" s="43"/>
@@ -11102,7 +11111,7 @@
     </row>
     <row r="16" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="43"/>
@@ -11117,7 +11126,7 @@
     </row>
     <row r="17" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="43"/>
@@ -11132,7 +11141,7 @@
     </row>
     <row r="18" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="43"/>
@@ -11147,7 +11156,7 @@
     </row>
     <row r="19" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="43"/>
@@ -11206,6 +11215,9 @@
       <c r="B23" s="15"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
+      <c r="E23" s="16" t="s">
+        <v>79</v>
+      </c>
       <c r="Q23" s="16" t="s">
         <v>79</v>
       </c>
@@ -11251,16 +11263,12 @@
       <c r="E25" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="Q25" s="31" t="s">
-        <v>79</v>
-      </c>
+      <c r="Q25" s="31"/>
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
       <c r="T25" s="31"/>
       <c r="W25" s="21"/>
-      <c r="X25" s="31" t="s">
-        <v>79</v>
-      </c>
+      <c r="X25" s="31"/>
     </row>
     <row r="26" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
@@ -12436,7 +12444,7 @@
   <dimension ref="A1:K186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12457,7 +12465,7 @@
       </c>
       <c r="C1" s="58"/>
       <c r="D1" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>77</v>
@@ -12465,19 +12473,19 @@
     </row>
     <row r="2" spans="1:11" s="53" customFormat="1" ht="109" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D2" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="F2" s="52" t="s">
         <v>21</v>
@@ -12486,7 +12494,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I2" s="51" t="s">
         <v>29</v>
@@ -12563,7 +12571,7 @@
     </row>
     <row r="6" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="56"/>
@@ -12586,7 +12594,7 @@
     </row>
     <row r="7" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="57"/>
@@ -12600,7 +12608,7 @@
     </row>
     <row r="8" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="57"/>
@@ -12612,7 +12620,7 @@
     </row>
     <row r="9" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="57"/>
@@ -12624,7 +12632,7 @@
     </row>
     <row r="10" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="55"/>
@@ -12639,7 +12647,7 @@
     </row>
     <row r="11" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="56" t="s">
@@ -12658,7 +12666,7 @@
     </row>
     <row r="12" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="60" t="s">
@@ -12673,7 +12681,7 @@
     </row>
     <row r="13" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="56"/>
@@ -12686,7 +12694,7 @@
     </row>
     <row r="14" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="57"/>
@@ -14212,7 +14220,7 @@
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="67" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>48</v>
@@ -14697,21 +14705,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100693BD51F8350324485FD573DEA5308EA" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3a5ad946f0818aa27759232261042403">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bcfd11aa4d094f7496148c95fffd8c5">
     <xsd:element name="properties">
@@ -14825,17 +14818,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D067DD9C-4F21-4672-8F3E-4EC03A859A66}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14849,17 +14858,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D067DD9C-4F21-4672-8F3E-4EC03A859A66}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correctie in onderzoek bij nationaliteit
</commit_message>
<xml_diff>
--- a/features/in onderzoek.xlsx
+++ b/features/in onderzoek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/GitHub/Haal-Centraal-BRP-bevragen/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52857A13-2D74-864D-9792-9542DF167565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD134B9-EA8B-5448-AFD8-BCAFAD3CB3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 persoon" sheetId="4" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="271">
   <si>
     <t>API</t>
   </si>
@@ -1802,7 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -7229,7 +7229,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7270,7 +7270,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>79</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -7280,18 +7280,12 @@
       <c r="B4" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="5" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="20" t="s">
         <v>79</v>
       </c>
     </row>
@@ -10725,7 +10719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456F4B46-E245-DB4D-BC75-1E1265C64598}">
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
@@ -14705,6 +14699,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100693BD51F8350324485FD573DEA5308EA" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3a5ad946f0818aa27759232261042403">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bcfd11aa4d094f7496148c95fffd8c5">
     <xsd:element name="properties">
@@ -14818,22 +14827,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D067DD9C-4F21-4672-8F3E-4EC03A859A66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2CD40-074F-4B13-A731-DCA6003B0A5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14847,27 +14864,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2CD40-074F-4B13-A731-DCA6003B0A5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D067DD9C-4F21-4672-8F3E-4EC03A859A66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
verduidelijken en corrigeren inOnderzoek feature en sheet
- verwijderen onnodig complexe regels bij afgeleide gegevens
- verwijderen leeftijd kind (in sheet)
</commit_message>
<xml_diff>
--- a/features/in onderzoek.xlsx
+++ b/features/in onderzoek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/GitHub/Haal-Centraal-BRP-bevragen/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD134B9-EA8B-5448-AFD8-BCAFAD3CB3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38D5A37-004E-7240-9BAA-2548A4520E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="271">
   <si>
     <t>API</t>
   </si>
@@ -1210,7 +1210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1267,32 +1267,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1438,23 +1418,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5148,7 +5111,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="53" customFormat="1" ht="200" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="55" t="s">
         <v>255</v>
       </c>
       <c r="B2" s="51" t="s">
@@ -7229,7 +7192,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7270,7 +7233,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>252</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -7280,12 +7243,18 @@
       <c r="B4" s="15" t="s">
         <v>79</v>
       </c>
+      <c r="D4" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>79</v>
       </c>
     </row>
@@ -10123,7 +10092,7 @@
       <c r="E2" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="F2" s="63"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -12435,82 +12404,76 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K186"/>
+  <dimension ref="A1:J186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="61" customWidth="1"/>
-    <col min="4" max="4" width="5.5" style="6" customWidth="1"/>
-    <col min="5" max="8" width="5.5" style="7" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="6" customWidth="1"/>
-    <col min="10" max="11" width="5.5" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="12.5" style="7"/>
+    <col min="2" max="3" width="5.5" style="6" customWidth="1"/>
+    <col min="4" max="7" width="5.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.5" style="6" customWidth="1"/>
+    <col min="9" max="10" width="5.5" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="12.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="53" customFormat="1" ht="109" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="53" customFormat="1" ht="109" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
         <v>260</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>245</v>
-      </c>
-      <c r="D2" s="51" t="s">
+      <c r="C2" s="51" t="s">
         <v>20</v>
       </c>
+      <c r="D2" s="52" t="s">
+        <v>270</v>
+      </c>
       <c r="E2" s="52" t="s">
-        <v>270</v>
+        <v>21</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="H2" s="51" t="s">
         <v>29</v>
       </c>
+      <c r="I2" s="52" t="s">
+        <v>30</v>
+      </c>
       <c r="J2" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>157</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -12522,54 +12485,51 @@
       <c r="G3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>79</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="15"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>159</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>213</v>
       </c>
       <c r="B6" s="15"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>79</v>
       </c>
       <c r="E6" s="16" t="s">
@@ -12581,1608 +12541,1429 @@
       <c r="G6" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>214</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>215</v>
       </c>
       <c r="B8" s="19"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="19"/>
+      <c r="D8" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>216</v>
       </c>
       <c r="B9" s="19"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="19"/>
-      <c r="F9" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="19"/>
+      <c r="E9" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>217</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="19"/>
-      <c r="G10" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="30"/>
+      <c r="C10" s="19"/>
+      <c r="F10" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
       <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-    </row>
-    <row r="11" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>236</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="I11" s="15" t="s">
+      <c r="C11" s="15"/>
+      <c r="H11" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>79</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="K11" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>237</v>
       </c>
       <c r="B12" s="30"/>
-      <c r="C12" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="I12" s="30" t="s">
-        <v>79</v>
-      </c>
+      <c r="C12" s="19"/>
+      <c r="H12" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="31"/>
       <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>238</v>
       </c>
       <c r="B13" s="15"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="19"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="19"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>239</v>
       </c>
       <c r="B14" s="19"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="19"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="19"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-    </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="25"/>
       <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="19"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="19"/>
-      <c r="I19" s="11"/>
+      <c r="C19" s="19"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="19"/>
-      <c r="I21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="19"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="19"/>
-      <c r="I23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="19"/>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="16"/>
       <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-    </row>
-    <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="15"/>
-      <c r="I27" s="19"/>
+      <c r="C27" s="15"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-    </row>
-    <row r="28" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="19"/>
-      <c r="I28" s="11"/>
+      <c r="C28" s="19"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
       <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-    </row>
-    <row r="29" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="19"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="19"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="19"/>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="19"/>
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-    </row>
-    <row r="32" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-    </row>
-    <row r="33" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
       <c r="B33" s="19"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-    </row>
-    <row r="34" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
       <c r="B34" s="19"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="16"/>
       <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-    </row>
-    <row r="35" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="19"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="19"/>
-      <c r="I36" s="15"/>
+      <c r="C36" s="19"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
       <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-    </row>
-    <row r="37" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="B37" s="15"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="20"/>
       <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-    </row>
-    <row r="38" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="19"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="19"/>
-    </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="19"/>
+    </row>
+    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
       <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-    </row>
-    <row r="40" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="B40" s="15"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="42"/>
       <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-    </row>
-    <row r="41" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="19"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="42"/>
       <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-    </row>
-    <row r="42" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="B42" s="15"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
       <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="42"/>
       <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-    </row>
-    <row r="43" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="19"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="19"/>
-      <c r="I43" s="41"/>
+      <c r="C43" s="19"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="42"/>
       <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-    </row>
-    <row r="44" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
       <c r="B44" s="19"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="16"/>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="42"/>
-      <c r="K44" s="42"/>
-    </row>
-    <row r="45" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="42"/>
       <c r="F45" s="42"/>
       <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="42"/>
       <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-    </row>
-    <row r="46" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="19"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="42"/>
       <c r="E46" s="42"/>
       <c r="F46" s="42"/>
       <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="42"/>
       <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-    </row>
-    <row r="47" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="42"/>
       <c r="E47" s="42"/>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="42"/>
       <c r="J47" s="42"/>
-      <c r="K47" s="42"/>
-    </row>
-    <row r="48" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="19"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42"/>
       <c r="E48" s="42"/>
       <c r="F48" s="42"/>
       <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="42"/>
       <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-    </row>
-    <row r="49" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="15"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="42"/>
       <c r="E49" s="42"/>
       <c r="F49" s="42"/>
       <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="42"/>
       <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-    </row>
-    <row r="50" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18"/>
       <c r="B50" s="19"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="42"/>
       <c r="E50" s="42"/>
       <c r="F50" s="42"/>
       <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="16"/>
       <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-    </row>
-    <row r="51" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18"/>
       <c r="B51" s="19"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="42"/>
       <c r="E51" s="42"/>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="19"/>
-    </row>
-    <row r="52" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H51" s="19"/>
+    </row>
+    <row r="52" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
       <c r="B52" s="19"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="42"/>
       <c r="E52" s="42"/>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="16"/>
       <c r="J52" s="16"/>
-      <c r="K52" s="16"/>
-    </row>
-    <row r="53" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
       <c r="B53" s="19"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="42"/>
       <c r="E53" s="42"/>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="19"/>
-    </row>
-    <row r="54" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="18"/>
       <c r="B54" s="19"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="41"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="42"/>
       <c r="E54" s="42"/>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="19"/>
-    </row>
-    <row r="55" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H54" s="19"/>
+    </row>
+    <row r="55" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="15"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="15"/>
-      <c r="I55" s="19"/>
+      <c r="C55" s="15"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="20"/>
       <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-    </row>
-    <row r="56" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18"/>
       <c r="B56" s="19"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="19"/>
-      <c r="I56" s="19"/>
-    </row>
-    <row r="57" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="19"/>
+      <c r="H56" s="19"/>
+    </row>
+    <row r="57" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
       <c r="B57" s="19"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="16"/>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="19"/>
-    </row>
-    <row r="58" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H57" s="19"/>
+    </row>
+    <row r="58" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="15"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="20"/>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18"/>
       <c r="B59" s="19"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="19"/>
-      <c r="I59" s="19"/>
-    </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="19"/>
+      <c r="H59" s="19"/>
+    </row>
+    <row r="60" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
       <c r="B60" s="11"/>
-      <c r="C60" s="55"/>
-      <c r="D60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="20"/>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
       <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="20"/>
       <c r="J60" s="20"/>
-      <c r="K60" s="20"/>
-    </row>
-    <row r="61" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
       <c r="B61" s="15"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="20"/>
       <c r="E61" s="20"/>
       <c r="F61" s="20"/>
       <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="15"/>
-    </row>
-    <row r="62" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="18"/>
       <c r="B62" s="19"/>
-      <c r="C62" s="57"/>
-      <c r="D62" s="19"/>
-      <c r="I62" s="19"/>
-    </row>
-    <row r="63" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="19"/>
+      <c r="H62" s="19"/>
+    </row>
+    <row r="63" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="18"/>
       <c r="B63" s="19"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="16"/>
       <c r="E63" s="16"/>
       <c r="F63" s="16"/>
       <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="12"/>
       <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-    </row>
-    <row r="64" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="18"/>
       <c r="B64" s="19"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="19"/>
-      <c r="I64" s="15"/>
+      <c r="C64" s="19"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="16"/>
       <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-    </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="55"/>
-      <c r="D65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
-      <c r="H65" s="20"/>
-      <c r="I65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="20"/>
       <c r="J65" s="20"/>
-      <c r="K65" s="20"/>
-    </row>
-    <row r="66" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="15"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="15"/>
-      <c r="I66" s="19"/>
+      <c r="C66" s="15"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="20"/>
       <c r="J66" s="20"/>
-      <c r="K66" s="20"/>
-    </row>
-    <row r="67" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="18"/>
       <c r="B67" s="19"/>
-      <c r="C67" s="57"/>
-      <c r="D67" s="19"/>
-      <c r="I67" s="19"/>
-    </row>
-    <row r="68" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="19"/>
+      <c r="H67" s="19"/>
+    </row>
+    <row r="68" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14"/>
       <c r="B68" s="15"/>
-      <c r="C68" s="56"/>
-      <c r="D68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="12"/>
       <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-    </row>
-    <row r="69" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="18"/>
       <c r="B69" s="19"/>
-      <c r="C69" s="57"/>
-      <c r="D69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="16"/>
       <c r="E69" s="16"/>
       <c r="F69" s="16"/>
       <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="16"/>
       <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
-    </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="10"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
       <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="20"/>
       <c r="J70" s="20"/>
-      <c r="K70" s="20"/>
-    </row>
-    <row r="71" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14"/>
       <c r="B71" s="15"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
       <c r="G71" s="20"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="15"/>
-    </row>
-    <row r="72" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H71" s="15"/>
+    </row>
+    <row r="72" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="18"/>
       <c r="B72" s="19"/>
-      <c r="C72" s="57"/>
-      <c r="D72" s="19"/>
-      <c r="I72" s="19"/>
-    </row>
-    <row r="73" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="19"/>
+      <c r="H72" s="19"/>
+    </row>
+    <row r="73" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="18"/>
       <c r="B73" s="19"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="12"/>
       <c r="J73" s="12"/>
-      <c r="K73" s="12"/>
-    </row>
-    <row r="74" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14"/>
       <c r="B74" s="15"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="15"/>
-      <c r="I74" s="15"/>
-    </row>
-    <row r="75" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="15"/>
+      <c r="H74" s="15"/>
+    </row>
+    <row r="75" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="18"/>
       <c r="B75" s="19"/>
-      <c r="C75" s="57"/>
-      <c r="D75" s="19"/>
-      <c r="I75" s="19"/>
-    </row>
-    <row r="76" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="19"/>
+      <c r="H75" s="19"/>
+    </row>
+    <row r="76" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="14"/>
       <c r="B76" s="15"/>
-      <c r="C76" s="56"/>
-      <c r="D76" s="15"/>
-      <c r="I76" s="19"/>
+      <c r="C76" s="15"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="20"/>
       <c r="J76" s="20"/>
-      <c r="K76" s="20"/>
-    </row>
-    <row r="77" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="18"/>
       <c r="B77" s="19"/>
-      <c r="C77" s="57"/>
-      <c r="D77" s="19"/>
-      <c r="I77" s="15"/>
+      <c r="C77" s="19"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="16"/>
       <c r="J77" s="16"/>
-      <c r="K77" s="16"/>
-    </row>
-    <row r="78" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="18"/>
       <c r="B78" s="19"/>
-      <c r="C78" s="57"/>
-      <c r="D78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="12"/>
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="19"/>
-    </row>
-    <row r="79" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H78" s="19"/>
+    </row>
+    <row r="79" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="18"/>
       <c r="B79" s="19"/>
-      <c r="C79" s="57"/>
-      <c r="D79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="16"/>
       <c r="E79" s="16"/>
       <c r="F79" s="16"/>
       <c r="G79" s="16"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="16"/>
       <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-    </row>
-    <row r="80" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="18"/>
       <c r="B80" s="19"/>
-      <c r="C80" s="57"/>
-      <c r="D80" s="19"/>
-      <c r="I80" s="19"/>
-    </row>
-    <row r="81" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C80" s="19"/>
+      <c r="H80" s="19"/>
+    </row>
+    <row r="81" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="18"/>
       <c r="B81" s="19"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="19"/>
-      <c r="I81" s="19"/>
-    </row>
-    <row r="82" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C81" s="19"/>
+      <c r="H81" s="19"/>
+    </row>
+    <row r="82" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="18"/>
       <c r="B82" s="19"/>
-      <c r="C82" s="57"/>
-      <c r="D82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="16"/>
       <c r="E82" s="16"/>
       <c r="F82" s="16"/>
       <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="19"/>
-    </row>
-    <row r="83" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H82" s="19"/>
+    </row>
+    <row r="83" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="18"/>
       <c r="B83" s="19"/>
-      <c r="C83" s="57"/>
-      <c r="D83" s="19"/>
-      <c r="I83" s="19"/>
-    </row>
-    <row r="84" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C83" s="19"/>
+      <c r="H83" s="19"/>
+    </row>
+    <row r="84" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="18"/>
       <c r="B84" s="19"/>
-      <c r="C84" s="57"/>
-      <c r="D84" s="15"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="16"/>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
       <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="19"/>
-    </row>
-    <row r="85" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H84" s="19"/>
+    </row>
+    <row r="85" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="18"/>
       <c r="B85" s="19"/>
-      <c r="C85" s="57"/>
-      <c r="D85" s="19"/>
-      <c r="I85" s="19"/>
-    </row>
-    <row r="86" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C85" s="19"/>
+      <c r="H85" s="19"/>
+    </row>
+    <row r="86" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="18"/>
       <c r="B86" s="19"/>
-      <c r="C86" s="57"/>
-      <c r="D86" s="19"/>
-      <c r="I86" s="19"/>
-    </row>
-    <row r="87" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C86" s="19"/>
+      <c r="H86" s="19"/>
+    </row>
+    <row r="87" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="18"/>
       <c r="B87" s="19"/>
-      <c r="C87" s="57"/>
-      <c r="D87" s="19"/>
-      <c r="I87" s="19"/>
-    </row>
-    <row r="88" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C87" s="19"/>
+      <c r="H87" s="19"/>
+    </row>
+    <row r="88" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="18"/>
       <c r="B88" s="19"/>
-      <c r="C88" s="57"/>
-      <c r="D88" s="19"/>
-      <c r="I88" s="19"/>
-    </row>
-    <row r="89" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C88" s="19"/>
+      <c r="H88" s="19"/>
+    </row>
+    <row r="89" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="18"/>
       <c r="B89" s="19"/>
-      <c r="C89" s="57"/>
-      <c r="D89" s="19"/>
-      <c r="I89" s="19"/>
-    </row>
-    <row r="90" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C89" s="19"/>
+      <c r="H89" s="19"/>
+    </row>
+    <row r="90" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18"/>
       <c r="B90" s="19"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="19"/>
-      <c r="I90" s="19"/>
-    </row>
-    <row r="91" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C90" s="19"/>
+      <c r="H90" s="19"/>
+    </row>
+    <row r="91" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18"/>
       <c r="B91" s="19"/>
-      <c r="C91" s="57"/>
-      <c r="D91" s="19"/>
-      <c r="I91" s="19"/>
-    </row>
-    <row r="92" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C91" s="19"/>
+      <c r="H91" s="19"/>
+    </row>
+    <row r="92" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="18"/>
       <c r="B92" s="19"/>
-      <c r="C92" s="57"/>
-      <c r="D92" s="19"/>
-      <c r="I92" s="19"/>
-    </row>
-    <row r="93" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C92" s="19"/>
+      <c r="H92" s="19"/>
+    </row>
+    <row r="93" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="18"/>
       <c r="B93" s="19"/>
-      <c r="C93" s="57"/>
-      <c r="D93" s="19"/>
-      <c r="I93" s="19"/>
-    </row>
-    <row r="94" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C93" s="19"/>
+      <c r="H93" s="19"/>
+    </row>
+    <row r="94" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="18"/>
       <c r="B94" s="19"/>
-      <c r="C94" s="57"/>
-      <c r="D94" s="19"/>
-      <c r="I94" s="19"/>
-    </row>
-    <row r="95" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C94" s="19"/>
+      <c r="H94" s="19"/>
+    </row>
+    <row r="95" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="18"/>
       <c r="B95" s="19"/>
-      <c r="C95" s="57"/>
-      <c r="D95" s="19"/>
-      <c r="I95" s="19"/>
-    </row>
-    <row r="96" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C95" s="19"/>
+      <c r="H95" s="19"/>
+    </row>
+    <row r="96" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="18"/>
       <c r="B96" s="19"/>
-      <c r="C96" s="57"/>
-      <c r="D96" s="19"/>
-      <c r="I96" s="19"/>
-    </row>
-    <row r="97" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C96" s="19"/>
+      <c r="H96" s="19"/>
+    </row>
+    <row r="97" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="18"/>
       <c r="B97" s="19"/>
-      <c r="C97" s="57"/>
-      <c r="D97" s="19"/>
-      <c r="I97" s="19"/>
-    </row>
-    <row r="98" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C97" s="19"/>
+      <c r="H97" s="19"/>
+    </row>
+    <row r="98" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="18"/>
       <c r="B98" s="19"/>
-      <c r="C98" s="57"/>
-      <c r="D98" s="19"/>
-      <c r="I98" s="19"/>
-    </row>
-    <row r="99" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C98" s="19"/>
+      <c r="H98" s="19"/>
+    </row>
+    <row r="99" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="18"/>
       <c r="B99" s="19"/>
-      <c r="C99" s="57"/>
-      <c r="D99" s="19"/>
-      <c r="I99" s="19"/>
-    </row>
-    <row r="100" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C99" s="19"/>
+      <c r="H99" s="19"/>
+    </row>
+    <row r="100" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="18"/>
       <c r="B100" s="19"/>
-      <c r="C100" s="57"/>
-      <c r="D100" s="19"/>
-      <c r="I100" s="19"/>
-    </row>
-    <row r="101" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C100" s="19"/>
+      <c r="H100" s="19"/>
+    </row>
+    <row r="101" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="18"/>
       <c r="B101" s="19"/>
-      <c r="C101" s="57"/>
-      <c r="D101" s="19"/>
-      <c r="I101" s="19"/>
-    </row>
-    <row r="102" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C101" s="19"/>
+      <c r="H101" s="19"/>
+    </row>
+    <row r="102" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="18"/>
       <c r="B102" s="19"/>
-      <c r="C102" s="57"/>
-      <c r="D102" s="19"/>
-      <c r="I102" s="19"/>
-    </row>
-    <row r="103" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C102" s="19"/>
+      <c r="H102" s="19"/>
+    </row>
+    <row r="103" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="18"/>
       <c r="B103" s="19"/>
-      <c r="C103" s="57"/>
-      <c r="D103" s="19"/>
-      <c r="I103" s="19"/>
-    </row>
-    <row r="104" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C103" s="19"/>
+      <c r="H103" s="19"/>
+    </row>
+    <row r="104" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="18"/>
       <c r="B104" s="19"/>
-      <c r="C104" s="57"/>
-      <c r="D104" s="19"/>
-      <c r="I104" s="19"/>
-    </row>
-    <row r="105" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C104" s="19"/>
+      <c r="H104" s="19"/>
+    </row>
+    <row r="105" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="18"/>
       <c r="B105" s="19"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="19"/>
-      <c r="I105" s="19"/>
-    </row>
-    <row r="106" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C105" s="19"/>
+      <c r="H105" s="19"/>
+    </row>
+    <row r="106" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="18"/>
       <c r="B106" s="19"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="19"/>
-      <c r="I106" s="19"/>
-    </row>
-    <row r="107" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C106" s="19"/>
+      <c r="H106" s="19"/>
+    </row>
+    <row r="107" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="18"/>
       <c r="B107" s="19"/>
-      <c r="C107" s="57"/>
-      <c r="D107" s="19"/>
-      <c r="I107" s="19"/>
-    </row>
-    <row r="108" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C107" s="19"/>
+      <c r="H107" s="19"/>
+    </row>
+    <row r="108" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="18"/>
       <c r="B108" s="19"/>
-      <c r="C108" s="57"/>
-      <c r="D108" s="19"/>
-      <c r="I108" s="19"/>
-    </row>
-    <row r="109" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C108" s="19"/>
+      <c r="H108" s="19"/>
+    </row>
+    <row r="109" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="18"/>
       <c r="B109" s="19"/>
-      <c r="C109" s="57"/>
-      <c r="D109" s="19"/>
-      <c r="I109" s="19"/>
-    </row>
-    <row r="110" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C109" s="19"/>
+      <c r="H109" s="19"/>
+    </row>
+    <row r="110" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="18"/>
       <c r="B110" s="19"/>
-      <c r="C110" s="57"/>
-      <c r="D110" s="19"/>
-      <c r="I110" s="19"/>
-    </row>
-    <row r="111" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C110" s="19"/>
+      <c r="H110" s="19"/>
+    </row>
+    <row r="111" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="18"/>
       <c r="B111" s="19"/>
-      <c r="C111" s="57"/>
-      <c r="D111" s="19"/>
-      <c r="I111" s="19"/>
-    </row>
-    <row r="112" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C111" s="19"/>
+      <c r="H111" s="19"/>
+    </row>
+    <row r="112" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="18"/>
       <c r="B112" s="19"/>
-      <c r="C112" s="57"/>
-      <c r="D112" s="19"/>
-      <c r="I112" s="19"/>
-    </row>
-    <row r="113" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C112" s="19"/>
+      <c r="H112" s="19"/>
+    </row>
+    <row r="113" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="18"/>
       <c r="B113" s="19"/>
-      <c r="C113" s="57"/>
-      <c r="D113" s="19"/>
-      <c r="I113" s="19"/>
-    </row>
-    <row r="114" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C113" s="19"/>
+      <c r="H113" s="19"/>
+    </row>
+    <row r="114" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="18"/>
       <c r="B114" s="19"/>
-      <c r="C114" s="57"/>
-      <c r="D114" s="19"/>
-      <c r="I114" s="19"/>
-    </row>
-    <row r="115" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C114" s="19"/>
+      <c r="H114" s="19"/>
+    </row>
+    <row r="115" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="18"/>
       <c r="B115" s="19"/>
-      <c r="C115" s="57"/>
-      <c r="D115" s="19"/>
-      <c r="I115" s="19"/>
-    </row>
-    <row r="116" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C115" s="19"/>
+      <c r="H115" s="19"/>
+    </row>
+    <row r="116" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="18"/>
       <c r="B116" s="19"/>
-      <c r="C116" s="57"/>
-      <c r="D116" s="19"/>
-      <c r="I116" s="19"/>
-    </row>
-    <row r="117" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C116" s="19"/>
+      <c r="H116" s="19"/>
+    </row>
+    <row r="117" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="18"/>
       <c r="B117" s="19"/>
-      <c r="C117" s="57"/>
-      <c r="D117" s="19"/>
-      <c r="I117" s="19"/>
-    </row>
-    <row r="118" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C117" s="19"/>
+      <c r="H117" s="19"/>
+    </row>
+    <row r="118" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="18"/>
       <c r="B118" s="19"/>
-      <c r="C118" s="57"/>
-      <c r="D118" s="19"/>
-      <c r="I118" s="19"/>
-    </row>
-    <row r="119" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C118" s="19"/>
+      <c r="H118" s="19"/>
+    </row>
+    <row r="119" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="18"/>
       <c r="B119" s="19"/>
-      <c r="C119" s="57"/>
-      <c r="D119" s="19"/>
-      <c r="I119" s="19"/>
-    </row>
-    <row r="120" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C119" s="19"/>
+      <c r="H119" s="19"/>
+    </row>
+    <row r="120" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="18"/>
       <c r="B120" s="19"/>
-      <c r="C120" s="57"/>
-      <c r="D120" s="19"/>
-      <c r="I120" s="19"/>
-    </row>
-    <row r="121" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C120" s="19"/>
+      <c r="H120" s="19"/>
+    </row>
+    <row r="121" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="18"/>
       <c r="B121" s="19"/>
-      <c r="C121" s="57"/>
-      <c r="D121" s="19"/>
-      <c r="I121" s="19"/>
-    </row>
-    <row r="122" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C121" s="19"/>
+      <c r="H121" s="19"/>
+    </row>
+    <row r="122" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="18"/>
       <c r="B122" s="19"/>
-      <c r="C122" s="57"/>
-      <c r="D122" s="19"/>
-      <c r="I122" s="19"/>
-    </row>
-    <row r="123" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C122" s="19"/>
+      <c r="H122" s="19"/>
+    </row>
+    <row r="123" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="18"/>
       <c r="B123" s="19"/>
-      <c r="C123" s="57"/>
-      <c r="D123" s="19"/>
-      <c r="I123" s="19"/>
-    </row>
-    <row r="124" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C123" s="19"/>
+      <c r="H123" s="19"/>
+    </row>
+    <row r="124" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="18"/>
       <c r="B124" s="19"/>
-      <c r="C124" s="57"/>
-      <c r="D124" s="19"/>
-      <c r="I124" s="19"/>
-    </row>
-    <row r="125" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C124" s="19"/>
+      <c r="H124" s="19"/>
+    </row>
+    <row r="125" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="18"/>
       <c r="B125" s="19"/>
-      <c r="C125" s="57"/>
-      <c r="D125" s="19"/>
-      <c r="I125" s="19"/>
-    </row>
-    <row r="126" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C125" s="19"/>
+      <c r="H125" s="19"/>
+    </row>
+    <row r="126" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="18"/>
       <c r="B126" s="19"/>
-      <c r="C126" s="57"/>
-      <c r="D126" s="19"/>
-      <c r="I126" s="19"/>
-    </row>
-    <row r="127" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C126" s="19"/>
+      <c r="H126" s="19"/>
+    </row>
+    <row r="127" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="18"/>
       <c r="B127" s="19"/>
-      <c r="C127" s="57"/>
-      <c r="D127" s="19"/>
-      <c r="I127" s="19"/>
-    </row>
-    <row r="128" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C127" s="19"/>
+      <c r="H127" s="19"/>
+    </row>
+    <row r="128" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="18"/>
       <c r="B128" s="19"/>
-      <c r="C128" s="57"/>
-      <c r="D128" s="19"/>
-      <c r="I128" s="19"/>
-    </row>
-    <row r="129" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C128" s="19"/>
+      <c r="H128" s="19"/>
+    </row>
+    <row r="129" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="18"/>
       <c r="B129" s="19"/>
-      <c r="C129" s="57"/>
-      <c r="D129" s="19"/>
-      <c r="I129" s="19"/>
-    </row>
-    <row r="130" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C129" s="19"/>
+      <c r="H129" s="19"/>
+    </row>
+    <row r="130" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="18"/>
       <c r="B130" s="19"/>
-      <c r="C130" s="57"/>
-      <c r="D130" s="19"/>
-      <c r="I130" s="19"/>
-    </row>
-    <row r="131" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C130" s="19"/>
+      <c r="H130" s="19"/>
+    </row>
+    <row r="131" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="18"/>
       <c r="B131" s="19"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="19"/>
-      <c r="I131" s="19"/>
-    </row>
-    <row r="132" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C131" s="19"/>
+      <c r="H131" s="19"/>
+    </row>
+    <row r="132" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="18"/>
       <c r="B132" s="19"/>
-      <c r="C132" s="57"/>
-      <c r="D132" s="19"/>
-      <c r="I132" s="19"/>
-    </row>
-    <row r="133" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C132" s="19"/>
+      <c r="H132" s="19"/>
+    </row>
+    <row r="133" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="18"/>
       <c r="B133" s="19"/>
-      <c r="C133" s="57"/>
-      <c r="D133" s="19"/>
-      <c r="I133" s="19"/>
-    </row>
-    <row r="134" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C133" s="19"/>
+      <c r="H133" s="19"/>
+    </row>
+    <row r="134" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="18"/>
       <c r="B134" s="19"/>
-      <c r="C134" s="57"/>
-      <c r="D134" s="19"/>
-      <c r="I134" s="19"/>
-    </row>
-    <row r="135" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C134" s="19"/>
+      <c r="H134" s="19"/>
+    </row>
+    <row r="135" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="18"/>
       <c r="B135" s="19"/>
-      <c r="C135" s="57"/>
-      <c r="D135" s="19"/>
-      <c r="I135" s="19"/>
-    </row>
-    <row r="136" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C135" s="19"/>
+      <c r="H135" s="19"/>
+    </row>
+    <row r="136" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="18"/>
       <c r="B136" s="19"/>
-      <c r="C136" s="57"/>
-      <c r="D136" s="19"/>
-      <c r="I136" s="19"/>
-    </row>
-    <row r="137" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C136" s="19"/>
+      <c r="H136" s="19"/>
+    </row>
+    <row r="137" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="18"/>
       <c r="B137" s="19"/>
-      <c r="C137" s="57"/>
-      <c r="D137" s="19"/>
-      <c r="I137" s="19"/>
-    </row>
-    <row r="138" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C137" s="19"/>
+      <c r="H137" s="19"/>
+    </row>
+    <row r="138" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="18"/>
       <c r="B138" s="19"/>
-      <c r="C138" s="57"/>
-      <c r="D138" s="19"/>
-      <c r="I138" s="19"/>
-    </row>
-    <row r="139" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C138" s="19"/>
+      <c r="H138" s="19"/>
+    </row>
+    <row r="139" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="18"/>
       <c r="B139" s="19"/>
-      <c r="C139" s="57"/>
-      <c r="D139" s="19"/>
-      <c r="I139" s="19"/>
-    </row>
-    <row r="140" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C139" s="19"/>
+      <c r="H139" s="19"/>
+    </row>
+    <row r="140" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="18"/>
       <c r="B140" s="19"/>
-      <c r="C140" s="57"/>
-      <c r="D140" s="19"/>
-      <c r="I140" s="19"/>
-    </row>
-    <row r="141" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C140" s="19"/>
+      <c r="H140" s="19"/>
+    </row>
+    <row r="141" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="18"/>
       <c r="B141" s="19"/>
-      <c r="C141" s="57"/>
-      <c r="D141" s="19"/>
-      <c r="I141" s="19"/>
-    </row>
-    <row r="142" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C141" s="19"/>
+      <c r="H141" s="19"/>
+    </row>
+    <row r="142" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="18"/>
       <c r="B142" s="19"/>
-      <c r="C142" s="57"/>
-      <c r="D142" s="19"/>
-      <c r="I142" s="19"/>
-    </row>
-    <row r="143" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C142" s="19"/>
+      <c r="H142" s="19"/>
+    </row>
+    <row r="143" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="18"/>
       <c r="B143" s="19"/>
-      <c r="C143" s="57"/>
-      <c r="D143" s="19"/>
-      <c r="I143" s="19"/>
-    </row>
-    <row r="144" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C143" s="19"/>
+      <c r="H143" s="19"/>
+    </row>
+    <row r="144" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="18"/>
       <c r="B144" s="19"/>
-      <c r="C144" s="57"/>
-      <c r="D144" s="19"/>
-      <c r="I144" s="19"/>
-    </row>
-    <row r="145" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C144" s="19"/>
+      <c r="H144" s="19"/>
+    </row>
+    <row r="145" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="18"/>
       <c r="B145" s="19"/>
-      <c r="C145" s="57"/>
-      <c r="D145" s="19"/>
-      <c r="I145" s="19"/>
-    </row>
-    <row r="146" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C145" s="19"/>
+      <c r="H145" s="19"/>
+    </row>
+    <row r="146" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="18"/>
       <c r="B146" s="19"/>
-      <c r="C146" s="57"/>
-      <c r="D146" s="19"/>
-      <c r="I146" s="19"/>
-    </row>
-    <row r="147" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C146" s="19"/>
+      <c r="H146" s="19"/>
+    </row>
+    <row r="147" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="18"/>
       <c r="B147" s="19"/>
-      <c r="C147" s="57"/>
-      <c r="D147" s="19"/>
-      <c r="I147" s="19"/>
-    </row>
-    <row r="148" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C147" s="19"/>
+      <c r="H147" s="19"/>
+    </row>
+    <row r="148" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="18"/>
       <c r="B148" s="19"/>
-      <c r="C148" s="57"/>
-      <c r="D148" s="19"/>
-      <c r="I148" s="19"/>
-    </row>
-    <row r="149" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C148" s="19"/>
+      <c r="H148" s="19"/>
+    </row>
+    <row r="149" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="18"/>
       <c r="B149" s="19"/>
-      <c r="C149" s="57"/>
-      <c r="D149" s="19"/>
-      <c r="I149" s="19"/>
-    </row>
-    <row r="150" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C149" s="19"/>
+      <c r="H149" s="19"/>
+    </row>
+    <row r="150" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="18"/>
       <c r="B150" s="19"/>
-      <c r="C150" s="57"/>
-      <c r="D150" s="19"/>
-      <c r="I150" s="19"/>
-    </row>
-    <row r="151" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C150" s="19"/>
+      <c r="H150" s="19"/>
+    </row>
+    <row r="151" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="18"/>
       <c r="B151" s="19"/>
-      <c r="C151" s="57"/>
-      <c r="D151" s="19"/>
-      <c r="I151" s="19"/>
-    </row>
-    <row r="152" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C151" s="19"/>
+      <c r="H151" s="19"/>
+    </row>
+    <row r="152" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="18"/>
       <c r="B152" s="19"/>
-      <c r="C152" s="57"/>
-      <c r="D152" s="19"/>
-      <c r="I152" s="19"/>
-    </row>
-    <row r="153" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C152" s="19"/>
+      <c r="H152" s="19"/>
+    </row>
+    <row r="153" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="18"/>
       <c r="B153" s="19"/>
-      <c r="C153" s="57"/>
-      <c r="D153" s="19"/>
-      <c r="I153" s="19"/>
-    </row>
-    <row r="154" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C153" s="19"/>
+      <c r="H153" s="19"/>
+    </row>
+    <row r="154" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="18"/>
       <c r="B154" s="19"/>
-      <c r="C154" s="57"/>
-      <c r="D154" s="19"/>
-      <c r="I154" s="19"/>
-    </row>
-    <row r="155" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C154" s="19"/>
+      <c r="H154" s="19"/>
+    </row>
+    <row r="155" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="18"/>
       <c r="B155" s="19"/>
-      <c r="C155" s="57"/>
-      <c r="D155" s="19"/>
-      <c r="I155" s="19"/>
-    </row>
-    <row r="156" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C155" s="19"/>
+      <c r="H155" s="19"/>
+    </row>
+    <row r="156" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="18"/>
       <c r="B156" s="19"/>
-      <c r="C156" s="57"/>
-      <c r="D156" s="19"/>
-      <c r="I156" s="19"/>
-    </row>
-    <row r="157" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C156" s="19"/>
+      <c r="H156" s="19"/>
+    </row>
+    <row r="157" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="18"/>
       <c r="B157" s="19"/>
-      <c r="C157" s="57"/>
-      <c r="D157" s="19"/>
-      <c r="I157" s="19"/>
-    </row>
-    <row r="158" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C157" s="19"/>
+      <c r="H157" s="19"/>
+    </row>
+    <row r="158" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="18"/>
       <c r="B158" s="19"/>
-      <c r="C158" s="57"/>
-      <c r="D158" s="19"/>
-      <c r="I158" s="19"/>
-    </row>
-    <row r="159" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C158" s="19"/>
+      <c r="H158" s="19"/>
+    </row>
+    <row r="159" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="18"/>
       <c r="B159" s="19"/>
-      <c r="C159" s="57"/>
-      <c r="D159" s="19"/>
-      <c r="I159" s="19"/>
-    </row>
-    <row r="160" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C159" s="19"/>
+      <c r="H159" s="19"/>
+    </row>
+    <row r="160" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="18"/>
       <c r="B160" s="19"/>
-      <c r="C160" s="57"/>
-      <c r="D160" s="19"/>
-      <c r="I160" s="19"/>
-    </row>
-    <row r="161" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C160" s="19"/>
+      <c r="H160" s="19"/>
+    </row>
+    <row r="161" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="18"/>
       <c r="B161" s="19"/>
-      <c r="C161" s="57"/>
-      <c r="D161" s="19"/>
-      <c r="I161" s="19"/>
-    </row>
-    <row r="162" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C161" s="19"/>
+      <c r="H161" s="19"/>
+    </row>
+    <row r="162" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="18"/>
       <c r="B162" s="19"/>
-      <c r="C162" s="57"/>
-      <c r="D162" s="19"/>
-      <c r="I162" s="19"/>
-    </row>
-    <row r="163" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C162" s="19"/>
+      <c r="H162" s="19"/>
+    </row>
+    <row r="163" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="18"/>
       <c r="B163" s="19"/>
-      <c r="C163" s="57"/>
-      <c r="D163" s="19"/>
-      <c r="I163" s="19"/>
-    </row>
-    <row r="164" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C163" s="19"/>
+      <c r="H163" s="19"/>
+    </row>
+    <row r="164" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="18"/>
       <c r="B164" s="19"/>
-      <c r="C164" s="57"/>
-      <c r="D164" s="19"/>
-      <c r="I164" s="19"/>
-    </row>
-    <row r="165" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C164" s="19"/>
+      <c r="H164" s="19"/>
+    </row>
+    <row r="165" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="18"/>
       <c r="B165" s="19"/>
-      <c r="C165" s="57"/>
-      <c r="D165" s="19"/>
-      <c r="I165" s="19"/>
-    </row>
-    <row r="166" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C165" s="19"/>
+      <c r="H165" s="19"/>
+    </row>
+    <row r="166" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="18"/>
       <c r="B166" s="19"/>
-      <c r="C166" s="57"/>
-      <c r="D166" s="19"/>
-      <c r="I166" s="19"/>
-    </row>
-    <row r="167" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C166" s="19"/>
+      <c r="H166" s="19"/>
+    </row>
+    <row r="167" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="18"/>
       <c r="B167" s="19"/>
-      <c r="C167" s="57"/>
-      <c r="D167" s="19"/>
-      <c r="I167" s="19"/>
-    </row>
-    <row r="168" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C167" s="19"/>
+      <c r="H167" s="19"/>
+    </row>
+    <row r="168" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="18"/>
       <c r="B168" s="19"/>
-      <c r="C168" s="57"/>
-      <c r="D168" s="19"/>
-      <c r="I168" s="19"/>
-    </row>
-    <row r="169" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C168" s="19"/>
+      <c r="H168" s="19"/>
+    </row>
+    <row r="169" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="18"/>
       <c r="B169" s="19"/>
-      <c r="C169" s="57"/>
-      <c r="D169" s="19"/>
-      <c r="I169" s="19"/>
-    </row>
-    <row r="170" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C169" s="19"/>
+      <c r="H169" s="19"/>
+    </row>
+    <row r="170" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="18"/>
       <c r="B170" s="19"/>
-      <c r="C170" s="57"/>
-      <c r="D170" s="19"/>
-      <c r="I170" s="19"/>
-    </row>
-    <row r="171" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C170" s="19"/>
+      <c r="H170" s="19"/>
+    </row>
+    <row r="171" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="18"/>
       <c r="B171" s="19"/>
-      <c r="C171" s="57"/>
-      <c r="D171" s="19"/>
-      <c r="I171" s="19"/>
-    </row>
-    <row r="172" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C171" s="19"/>
+      <c r="H171" s="19"/>
+    </row>
+    <row r="172" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="18"/>
       <c r="B172" s="19"/>
-      <c r="C172" s="57"/>
-      <c r="D172" s="19"/>
-      <c r="I172" s="19"/>
-    </row>
-    <row r="173" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C172" s="19"/>
+      <c r="H172" s="19"/>
+    </row>
+    <row r="173" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="18"/>
       <c r="B173" s="19"/>
-      <c r="C173" s="57"/>
-      <c r="D173" s="19"/>
-      <c r="I173" s="19"/>
-    </row>
-    <row r="174" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C173" s="19"/>
+      <c r="H173" s="19"/>
+    </row>
+    <row r="174" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="18"/>
       <c r="B174" s="19"/>
-      <c r="C174" s="57"/>
-      <c r="D174" s="19"/>
-      <c r="I174" s="19"/>
-    </row>
-    <row r="175" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C174" s="19"/>
+      <c r="H174" s="19"/>
+    </row>
+    <row r="175" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="18"/>
       <c r="B175" s="19"/>
-      <c r="C175" s="57"/>
-      <c r="D175" s="19"/>
-      <c r="I175" s="19"/>
-    </row>
-    <row r="176" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C175" s="19"/>
+      <c r="H175" s="19"/>
+    </row>
+    <row r="176" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="18"/>
       <c r="B176" s="19"/>
-      <c r="C176" s="57"/>
-      <c r="D176" s="19"/>
-      <c r="I176" s="19"/>
-    </row>
-    <row r="177" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C176" s="19"/>
+      <c r="H176" s="19"/>
+    </row>
+    <row r="177" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="18"/>
       <c r="B177" s="19"/>
-      <c r="C177" s="57"/>
-      <c r="D177" s="19"/>
-      <c r="I177" s="19"/>
-    </row>
-    <row r="178" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C177" s="19"/>
+      <c r="H177" s="19"/>
+    </row>
+    <row r="178" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178" s="18"/>
       <c r="B178" s="19"/>
-      <c r="C178" s="57"/>
-      <c r="D178" s="19"/>
-      <c r="I178" s="19"/>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D179" s="19"/>
+      <c r="C178" s="19"/>
+      <c r="H178" s="19"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C179" s="19"/>
+      <c r="D179" s="20"/>
       <c r="E179" s="20"/>
       <c r="F179" s="20"/>
       <c r="G179" s="20"/>
-      <c r="H179" s="20"/>
-      <c r="I179" s="19"/>
+      <c r="H179" s="19"/>
+      <c r="I179" s="20"/>
       <c r="J179" s="20"/>
-      <c r="K179" s="20"/>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D180" s="19"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C180" s="19"/>
+      <c r="D180" s="20"/>
       <c r="E180" s="20"/>
       <c r="F180" s="20"/>
       <c r="G180" s="20"/>
-      <c r="H180" s="20"/>
-      <c r="I180" s="19"/>
+      <c r="H180" s="19"/>
+      <c r="I180" s="20"/>
       <c r="J180" s="20"/>
-      <c r="K180" s="20"/>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D181" s="19"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C181" s="19"/>
+      <c r="D181" s="20"/>
       <c r="E181" s="20"/>
       <c r="F181" s="20"/>
       <c r="G181" s="20"/>
-      <c r="H181" s="20"/>
-      <c r="I181" s="19"/>
+      <c r="H181" s="19"/>
+      <c r="I181" s="20"/>
       <c r="J181" s="20"/>
-      <c r="K181" s="20"/>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D182" s="19"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C182" s="19"/>
+      <c r="D182" s="20"/>
       <c r="E182" s="20"/>
       <c r="F182" s="20"/>
       <c r="G182" s="20"/>
-      <c r="H182" s="20"/>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D183" s="19"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C183" s="19"/>
+      <c r="D183" s="20"/>
       <c r="E183" s="20"/>
       <c r="F183" s="20"/>
       <c r="G183" s="20"/>
-      <c r="H183" s="20"/>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D184" s="19"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C184" s="19"/>
+      <c r="D184" s="20"/>
       <c r="E184" s="20"/>
       <c r="F184" s="20"/>
       <c r="G184" s="20"/>
-      <c r="H184" s="20"/>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D185" s="19"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C185" s="19"/>
+      <c r="D185" s="20"/>
       <c r="E185" s="20"/>
       <c r="F185" s="20"/>
       <c r="G185" s="20"/>
-      <c r="H185" s="20"/>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D186" s="19"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C186" s="19"/>
+      <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
       <c r="G186" s="20"/>
-      <c r="H186" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14699,21 +14480,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100693BD51F8350324485FD573DEA5308EA" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3a5ad946f0818aa27759232261042403">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bcfd11aa4d094f7496148c95fffd8c5">
     <xsd:element name="properties">
@@ -14827,7 +14593,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D067DD9C-4F21-4672-8F3E-4EC03A859A66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -14842,26 +14639,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2CD40-074F-4B13-A731-DCA6003B0A5A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
toevoegen leeswijzer aan sheet
</commit_message>
<xml_diff>
--- a/features/in onderzoek.xlsx
+++ b/features/in onderzoek.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/GitHub/Haal-Centraal-BRP-bevragen/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38D5A37-004E-7240-9BAA-2548A4520E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767FE8F4-A2A3-704F-9548-22BB5AB964F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1 persoon" sheetId="4" r:id="rId1"/>
-    <sheet name="RSGB" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="2 3 ouders" sheetId="5" r:id="rId3"/>
-    <sheet name="4 nationaliteit" sheetId="9" r:id="rId4"/>
-    <sheet name="5 partners" sheetId="3" r:id="rId5"/>
-    <sheet name="6 overlijden" sheetId="10" r:id="rId6"/>
-    <sheet name="8 verblijfplaats" sheetId="11" r:id="rId7"/>
-    <sheet name="9 kinderen" sheetId="7" r:id="rId8"/>
-    <sheet name="10 verblijfstitel" sheetId="12" r:id="rId9"/>
-    <sheet name="11 gezagsverhouding" sheetId="13" r:id="rId10"/>
-    <sheet name="12 reisdocumenten" sheetId="6" r:id="rId11"/>
+    <sheet name="leeswijzer" sheetId="14" r:id="rId1"/>
+    <sheet name="1 persoon" sheetId="4" r:id="rId2"/>
+    <sheet name="RSGB" sheetId="1" state="hidden" r:id="rId3"/>
+    <sheet name="2 3 ouders" sheetId="5" r:id="rId4"/>
+    <sheet name="4 nationaliteit" sheetId="9" r:id="rId5"/>
+    <sheet name="5 partners" sheetId="3" r:id="rId6"/>
+    <sheet name="6 overlijden" sheetId="10" r:id="rId7"/>
+    <sheet name="8 verblijfplaats" sheetId="11" r:id="rId8"/>
+    <sheet name="9 kinderen" sheetId="7" r:id="rId9"/>
+    <sheet name="10 verblijfstitel" sheetId="12" r:id="rId10"/>
+    <sheet name="11 gezagsverhouding" sheetId="13" r:id="rId11"/>
+    <sheet name="12 reisdocumenten" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -255,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="280">
   <si>
     <t>API</t>
   </si>
@@ -1069,6 +1070,33 @@
   </si>
   <si>
     <t>adellijkeTitelPredicaat</t>
+  </si>
+  <si>
+    <t>Leeswijzer</t>
+  </si>
+  <si>
+    <t>Per LO GBA categorie is er een sheet met de betreffende gegevens.</t>
+  </si>
+  <si>
+    <t>Dit document illustreert de werking vertaling van inOnderzoek van een LO GBA elementnummer naar een boolean in de Haal Centraal API.</t>
+  </si>
+  <si>
+    <t>De logica en werking hiervan is beschreven in het document "in_onderzoek.feature".</t>
+  </si>
+  <si>
+    <t>In rij 2 staan de namen van properties</t>
+  </si>
+  <si>
+    <t>In kolom A staan de LO GBA elementnummers, wat mogelijke waarden zijn voor in onderzoek (element 83.10) in de bron GBA-V.</t>
+  </si>
+  <si>
+    <t>Bij elke waarde (kolom A) staan in de volgende kolommen een "X" wanneer het betreffende property (rij 2) in inOnderzoek moet worden opgenomen (met waarde true).</t>
+  </si>
+  <si>
+    <t>De opgenomen waarden en "X" kunnen een kleur blauw hebben, wat betekent dat de waarde de hele categorie in onderzoek zet</t>
+  </si>
+  <si>
+    <t>De opgenomen waarden en "X" kunnen een kleur groen hebben, wat betekent dat de waarde een hele groep in onderzoek zet</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1424,6 +1452,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1762,10 +1791,1853 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4E145B-FFEB-B14F-8402-2F6CA11C9574}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="128.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C75824-A823-0940-8E8F-EA7B7D338F3B}">
+  <dimension ref="A1:D110"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
+    <col min="3" max="4" width="5.5" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="12.5" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="9" customFormat="1" ht="67" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="D6" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+    </row>
+    <row r="22" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+    </row>
+    <row r="27" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+    </row>
+    <row r="28" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+    </row>
+    <row r="29" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="19"/>
+    </row>
+    <row r="36" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+    </row>
+    <row r="38" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+    </row>
+    <row r="39" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
+    </row>
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18"/>
+      <c r="B40" s="19"/>
+    </row>
+    <row r="41" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18"/>
+      <c r="B42" s="19"/>
+    </row>
+    <row r="43" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+    </row>
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+    </row>
+    <row r="45" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+    </row>
+    <row r="46" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+    </row>
+    <row r="47" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="B47" s="19"/>
+    </row>
+    <row r="48" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="B48" s="19"/>
+    </row>
+    <row r="49" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="18"/>
+      <c r="B49" s="19"/>
+    </row>
+    <row r="50" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18"/>
+      <c r="B50" s="19"/>
+    </row>
+    <row r="51" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
+    </row>
+    <row r="52" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
+      <c r="B52" s="19"/>
+    </row>
+    <row r="53" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="18"/>
+      <c r="B55" s="19"/>
+    </row>
+    <row r="56" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="18"/>
+      <c r="B56" s="19"/>
+    </row>
+    <row r="57" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
+    </row>
+    <row r="58" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="18"/>
+      <c r="B58" s="19"/>
+    </row>
+    <row r="59" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
+    </row>
+    <row r="60" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="18"/>
+      <c r="B60" s="19"/>
+    </row>
+    <row r="61" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="18"/>
+      <c r="B61" s="19"/>
+    </row>
+    <row r="62" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="18"/>
+      <c r="B62" s="19"/>
+    </row>
+    <row r="63" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="18"/>
+      <c r="B63" s="19"/>
+    </row>
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="18"/>
+      <c r="B64" s="19"/>
+    </row>
+    <row r="65" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="18"/>
+      <c r="B65" s="19"/>
+    </row>
+    <row r="66" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="18"/>
+      <c r="B66" s="19"/>
+    </row>
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
+    </row>
+    <row r="68" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="18"/>
+      <c r="B68" s="19"/>
+    </row>
+    <row r="69" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="18"/>
+      <c r="B69" s="19"/>
+    </row>
+    <row r="70" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="18"/>
+      <c r="B70" s="19"/>
+    </row>
+    <row r="71" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="18"/>
+      <c r="B71" s="19"/>
+    </row>
+    <row r="72" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="18"/>
+      <c r="B72" s="19"/>
+    </row>
+    <row r="73" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+    </row>
+    <row r="74" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="18"/>
+      <c r="B74" s="19"/>
+    </row>
+    <row r="75" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
+    </row>
+    <row r="76" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="18"/>
+      <c r="B76" s="19"/>
+    </row>
+    <row r="77" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="18"/>
+      <c r="B77" s="19"/>
+    </row>
+    <row r="78" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="18"/>
+      <c r="B78" s="19"/>
+    </row>
+    <row r="79" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="19"/>
+    </row>
+    <row r="80" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="18"/>
+      <c r="B80" s="19"/>
+    </row>
+    <row r="81" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="18"/>
+      <c r="B81" s="19"/>
+    </row>
+    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="18"/>
+      <c r="B82" s="19"/>
+    </row>
+    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="18"/>
+      <c r="B83" s="19"/>
+    </row>
+    <row r="84" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="18"/>
+      <c r="B84" s="19"/>
+    </row>
+    <row r="85" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="18"/>
+      <c r="B85" s="19"/>
+    </row>
+    <row r="86" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18"/>
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="18"/>
+      <c r="B87" s="19"/>
+    </row>
+    <row r="88" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18"/>
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="18"/>
+      <c r="B89" s="19"/>
+    </row>
+    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18"/>
+      <c r="B90" s="19"/>
+    </row>
+    <row r="91" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="18"/>
+      <c r="B91" s="19"/>
+    </row>
+    <row r="92" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="18"/>
+      <c r="B92" s="19"/>
+    </row>
+    <row r="93" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="18"/>
+      <c r="B94" s="19"/>
+    </row>
+    <row r="95" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="18"/>
+      <c r="B95" s="19"/>
+    </row>
+    <row r="96" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="18"/>
+      <c r="B96" s="19"/>
+    </row>
+    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19"/>
+    </row>
+    <row r="98" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19"/>
+    </row>
+    <row r="100" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19"/>
+    </row>
+    <row r="101" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19"/>
+    </row>
+    <row r="102" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19"/>
+    </row>
+    <row r="103" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="18"/>
+      <c r="B103" s="19"/>
+    </row>
+    <row r="104" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19"/>
+    </row>
+    <row r="105" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="18"/>
+      <c r="B105" s="19"/>
+    </row>
+    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="18"/>
+      <c r="B106" s="19"/>
+    </row>
+    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19"/>
+    </row>
+    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="18"/>
+      <c r="B108" s="19"/>
+    </row>
+    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="18"/>
+      <c r="B109" s="19"/>
+    </row>
+    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="18"/>
+      <c r="B110" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2B85B4-77BB-514B-878C-DDA4580BABC6}">
+  <dimension ref="A1:C110"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="12.5" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="9" customFormat="1" ht="133" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+    </row>
+    <row r="22" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+    </row>
+    <row r="27" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+    </row>
+    <row r="28" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+    </row>
+    <row r="29" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="19"/>
+    </row>
+    <row r="36" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+    </row>
+    <row r="38" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+    </row>
+    <row r="39" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
+    </row>
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18"/>
+      <c r="B40" s="19"/>
+    </row>
+    <row r="41" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18"/>
+      <c r="B42" s="19"/>
+    </row>
+    <row r="43" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+    </row>
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+    </row>
+    <row r="45" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+    </row>
+    <row r="46" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+    </row>
+    <row r="47" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="B47" s="19"/>
+    </row>
+    <row r="48" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="B48" s="19"/>
+    </row>
+    <row r="49" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="18"/>
+      <c r="B49" s="19"/>
+    </row>
+    <row r="50" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18"/>
+      <c r="B50" s="19"/>
+    </row>
+    <row r="51" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
+    </row>
+    <row r="52" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
+      <c r="B52" s="19"/>
+    </row>
+    <row r="53" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="18"/>
+      <c r="B55" s="19"/>
+    </row>
+    <row r="56" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="18"/>
+      <c r="B56" s="19"/>
+    </row>
+    <row r="57" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
+    </row>
+    <row r="58" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="18"/>
+      <c r="B58" s="19"/>
+    </row>
+    <row r="59" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
+    </row>
+    <row r="60" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="18"/>
+      <c r="B60" s="19"/>
+    </row>
+    <row r="61" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="18"/>
+      <c r="B61" s="19"/>
+    </row>
+    <row r="62" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="18"/>
+      <c r="B62" s="19"/>
+    </row>
+    <row r="63" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="18"/>
+      <c r="B63" s="19"/>
+    </row>
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="18"/>
+      <c r="B64" s="19"/>
+    </row>
+    <row r="65" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="18"/>
+      <c r="B65" s="19"/>
+    </row>
+    <row r="66" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="18"/>
+      <c r="B66" s="19"/>
+    </row>
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
+    </row>
+    <row r="68" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="18"/>
+      <c r="B68" s="19"/>
+    </row>
+    <row r="69" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="18"/>
+      <c r="B69" s="19"/>
+    </row>
+    <row r="70" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="18"/>
+      <c r="B70" s="19"/>
+    </row>
+    <row r="71" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="18"/>
+      <c r="B71" s="19"/>
+    </row>
+    <row r="72" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="18"/>
+      <c r="B72" s="19"/>
+    </row>
+    <row r="73" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+    </row>
+    <row r="74" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="18"/>
+      <c r="B74" s="19"/>
+    </row>
+    <row r="75" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
+    </row>
+    <row r="76" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="18"/>
+      <c r="B76" s="19"/>
+    </row>
+    <row r="77" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="18"/>
+      <c r="B77" s="19"/>
+    </row>
+    <row r="78" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="18"/>
+      <c r="B78" s="19"/>
+    </row>
+    <row r="79" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="19"/>
+    </row>
+    <row r="80" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="18"/>
+      <c r="B80" s="19"/>
+    </row>
+    <row r="81" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="18"/>
+      <c r="B81" s="19"/>
+    </row>
+    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="18"/>
+      <c r="B82" s="19"/>
+    </row>
+    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="18"/>
+      <c r="B83" s="19"/>
+    </row>
+    <row r="84" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="18"/>
+      <c r="B84" s="19"/>
+    </row>
+    <row r="85" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="18"/>
+      <c r="B85" s="19"/>
+    </row>
+    <row r="86" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18"/>
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="18"/>
+      <c r="B87" s="19"/>
+    </row>
+    <row r="88" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18"/>
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="18"/>
+      <c r="B89" s="19"/>
+    </row>
+    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18"/>
+      <c r="B90" s="19"/>
+    </row>
+    <row r="91" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="18"/>
+      <c r="B91" s="19"/>
+    </row>
+    <row r="92" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="18"/>
+      <c r="B92" s="19"/>
+    </row>
+    <row r="93" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="18"/>
+      <c r="B94" s="19"/>
+    </row>
+    <row r="95" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="18"/>
+      <c r="B95" s="19"/>
+    </row>
+    <row r="96" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="18"/>
+      <c r="B96" s="19"/>
+    </row>
+    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19"/>
+    </row>
+    <row r="98" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19"/>
+    </row>
+    <row r="100" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19"/>
+    </row>
+    <row r="101" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19"/>
+    </row>
+    <row r="102" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19"/>
+    </row>
+    <row r="103" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="18"/>
+      <c r="B103" s="19"/>
+    </row>
+    <row r="104" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19"/>
+    </row>
+    <row r="105" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="18"/>
+      <c r="B105" s="19"/>
+    </row>
+    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="18"/>
+      <c r="B106" s="19"/>
+    </row>
+    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19"/>
+    </row>
+    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="18"/>
+      <c r="B108" s="19"/>
+    </row>
+    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="18"/>
+      <c r="B109" s="19"/>
+    </row>
+    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="18"/>
+      <c r="B110" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:N178"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
+    <col min="3" max="9" width="5.5" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="12.5" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="9" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+    </row>
+    <row r="3" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="30"/>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="30"/>
+    </row>
+    <row r="13" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+    </row>
+    <row r="22" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+    </row>
+    <row r="29" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+    </row>
+    <row r="38" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+    </row>
+    <row r="39" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+    </row>
+    <row r="40" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+    </row>
+    <row r="41" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15"/>
+    </row>
+    <row r="43" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+    </row>
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+    </row>
+    <row r="45" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+    </row>
+    <row r="46" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+    </row>
+    <row r="47" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+    </row>
+    <row r="48" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="B48" s="19"/>
+    </row>
+    <row r="49" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+    </row>
+    <row r="50" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18"/>
+      <c r="B50" s="19"/>
+    </row>
+    <row r="51" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
+    </row>
+    <row r="52" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
+      <c r="B52" s="19"/>
+    </row>
+    <row r="53" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="18"/>
+      <c r="B56" s="19"/>
+    </row>
+    <row r="57" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
+    </row>
+    <row r="58" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" s="15"/>
+    </row>
+    <row r="59" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
+    </row>
+    <row r="60" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+    </row>
+    <row r="61" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="14"/>
+      <c r="B61" s="15"/>
+    </row>
+    <row r="62" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="18"/>
+      <c r="B62" s="19"/>
+    </row>
+    <row r="63" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="18"/>
+      <c r="B63" s="19"/>
+    </row>
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="18"/>
+      <c r="B64" s="19"/>
+    </row>
+    <row r="65" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
+    </row>
+    <row r="66" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="14"/>
+      <c r="B66" s="15"/>
+    </row>
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
+    </row>
+    <row r="68" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="15"/>
+    </row>
+    <row r="69" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="18"/>
+      <c r="B69" s="19"/>
+    </row>
+    <row r="70" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="10"/>
+      <c r="B70" s="11"/>
+    </row>
+    <row r="71" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14"/>
+      <c r="B71" s="15"/>
+    </row>
+    <row r="72" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="18"/>
+      <c r="B72" s="19"/>
+    </row>
+    <row r="73" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+    </row>
+    <row r="74" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
+      <c r="B74" s="15"/>
+    </row>
+    <row r="75" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
+    </row>
+    <row r="76" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="15"/>
+    </row>
+    <row r="77" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="18"/>
+      <c r="B77" s="19"/>
+    </row>
+    <row r="78" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="18"/>
+      <c r="B78" s="19"/>
+    </row>
+    <row r="79" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="19"/>
+    </row>
+    <row r="80" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="18"/>
+      <c r="B80" s="19"/>
+    </row>
+    <row r="81" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="18"/>
+      <c r="B81" s="19"/>
+    </row>
+    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="18"/>
+      <c r="B82" s="19"/>
+    </row>
+    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="18"/>
+      <c r="B83" s="19"/>
+    </row>
+    <row r="84" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="18"/>
+      <c r="B84" s="19"/>
+    </row>
+    <row r="85" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="18"/>
+      <c r="B85" s="19"/>
+    </row>
+    <row r="86" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18"/>
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="18"/>
+      <c r="B87" s="19"/>
+    </row>
+    <row r="88" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18"/>
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="18"/>
+      <c r="B89" s="19"/>
+    </row>
+    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18"/>
+      <c r="B90" s="19"/>
+    </row>
+    <row r="91" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="18"/>
+      <c r="B91" s="19"/>
+    </row>
+    <row r="92" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="18"/>
+      <c r="B92" s="19"/>
+    </row>
+    <row r="93" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="18"/>
+      <c r="B94" s="19"/>
+    </row>
+    <row r="95" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="18"/>
+      <c r="B95" s="19"/>
+    </row>
+    <row r="96" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="18"/>
+      <c r="B96" s="19"/>
+    </row>
+    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19"/>
+    </row>
+    <row r="98" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19"/>
+    </row>
+    <row r="100" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19"/>
+    </row>
+    <row r="101" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19"/>
+    </row>
+    <row r="102" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19"/>
+    </row>
+    <row r="103" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="18"/>
+      <c r="B103" s="19"/>
+    </row>
+    <row r="104" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19"/>
+    </row>
+    <row r="105" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="18"/>
+      <c r="B105" s="19"/>
+    </row>
+    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="18"/>
+      <c r="B106" s="19"/>
+    </row>
+    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19"/>
+    </row>
+    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="18"/>
+      <c r="B108" s="19"/>
+    </row>
+    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="18"/>
+      <c r="B109" s="19"/>
+    </row>
+    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="18"/>
+      <c r="B110" s="19"/>
+    </row>
+    <row r="111" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="18"/>
+      <c r="B111" s="19"/>
+    </row>
+    <row r="112" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="18"/>
+      <c r="B112" s="19"/>
+    </row>
+    <row r="113" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="18"/>
+      <c r="B113" s="19"/>
+    </row>
+    <row r="114" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="18"/>
+      <c r="B114" s="19"/>
+    </row>
+    <row r="115" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="18"/>
+      <c r="B115" s="19"/>
+    </row>
+    <row r="116" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="18"/>
+      <c r="B116" s="19"/>
+    </row>
+    <row r="117" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="18"/>
+      <c r="B117" s="19"/>
+    </row>
+    <row r="118" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="18"/>
+      <c r="B118" s="19"/>
+    </row>
+    <row r="119" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="18"/>
+      <c r="B119" s="19"/>
+    </row>
+    <row r="120" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="18"/>
+      <c r="B120" s="19"/>
+    </row>
+    <row r="121" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="18"/>
+      <c r="B121" s="19"/>
+    </row>
+    <row r="122" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="18"/>
+      <c r="B122" s="19"/>
+    </row>
+    <row r="123" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="18"/>
+      <c r="B123" s="19"/>
+    </row>
+    <row r="124" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="18"/>
+      <c r="B124" s="19"/>
+    </row>
+    <row r="125" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="18"/>
+      <c r="B125" s="19"/>
+    </row>
+    <row r="126" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="18"/>
+      <c r="B126" s="19"/>
+    </row>
+    <row r="127" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="18"/>
+      <c r="B127" s="19"/>
+    </row>
+    <row r="128" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="18"/>
+      <c r="B128" s="19"/>
+    </row>
+    <row r="129" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="18"/>
+      <c r="B129" s="19"/>
+    </row>
+    <row r="130" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="18"/>
+      <c r="B130" s="19"/>
+    </row>
+    <row r="131" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="18"/>
+      <c r="B131" s="19"/>
+    </row>
+    <row r="132" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="18"/>
+      <c r="B132" s="19"/>
+    </row>
+    <row r="133" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="18"/>
+      <c r="B133" s="19"/>
+    </row>
+    <row r="134" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="18"/>
+      <c r="B134" s="19"/>
+    </row>
+    <row r="135" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="18"/>
+      <c r="B135" s="19"/>
+    </row>
+    <row r="136" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="18"/>
+      <c r="B136" s="19"/>
+    </row>
+    <row r="137" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="18"/>
+      <c r="B137" s="19"/>
+    </row>
+    <row r="138" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="18"/>
+      <c r="B138" s="19"/>
+    </row>
+    <row r="139" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="18"/>
+      <c r="B139" s="19"/>
+    </row>
+    <row r="140" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="18"/>
+      <c r="B140" s="19"/>
+    </row>
+    <row r="141" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="18"/>
+      <c r="B141" s="19"/>
+    </row>
+    <row r="142" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="18"/>
+      <c r="B142" s="19"/>
+    </row>
+    <row r="143" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="18"/>
+      <c r="B143" s="19"/>
+    </row>
+    <row r="144" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="18"/>
+      <c r="B144" s="19"/>
+    </row>
+    <row r="145" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="18"/>
+      <c r="B145" s="19"/>
+    </row>
+    <row r="146" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="18"/>
+      <c r="B146" s="19"/>
+    </row>
+    <row r="147" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="18"/>
+      <c r="B147" s="19"/>
+    </row>
+    <row r="148" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="18"/>
+      <c r="B148" s="19"/>
+    </row>
+    <row r="149" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="18"/>
+      <c r="B149" s="19"/>
+    </row>
+    <row r="150" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="18"/>
+      <c r="B150" s="19"/>
+    </row>
+    <row r="151" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="18"/>
+      <c r="B151" s="19"/>
+    </row>
+    <row r="152" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="18"/>
+      <c r="B152" s="19"/>
+    </row>
+    <row r="153" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="18"/>
+      <c r="B153" s="19"/>
+    </row>
+    <row r="154" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="18"/>
+      <c r="B154" s="19"/>
+    </row>
+    <row r="155" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="18"/>
+      <c r="B155" s="19"/>
+    </row>
+    <row r="156" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="18"/>
+      <c r="B156" s="19"/>
+    </row>
+    <row r="157" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="18"/>
+      <c r="B157" s="19"/>
+    </row>
+    <row r="158" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="18"/>
+      <c r="B158" s="19"/>
+    </row>
+    <row r="159" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="18"/>
+      <c r="B159" s="19"/>
+    </row>
+    <row r="160" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="18"/>
+      <c r="B160" s="19"/>
+    </row>
+    <row r="161" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="18"/>
+      <c r="B161" s="19"/>
+    </row>
+    <row r="162" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="18"/>
+      <c r="B162" s="19"/>
+    </row>
+    <row r="163" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="18"/>
+      <c r="B163" s="19"/>
+    </row>
+    <row r="164" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="18"/>
+      <c r="B164" s="19"/>
+    </row>
+    <row r="165" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="18"/>
+      <c r="B165" s="19"/>
+    </row>
+    <row r="166" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="18"/>
+      <c r="B166" s="19"/>
+    </row>
+    <row r="167" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="18"/>
+      <c r="B167" s="19"/>
+    </row>
+    <row r="168" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="18"/>
+      <c r="B168" s="19"/>
+    </row>
+    <row r="169" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="18"/>
+      <c r="B169" s="19"/>
+    </row>
+    <row r="170" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="18"/>
+      <c r="B170" s="19"/>
+    </row>
+    <row r="171" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="18"/>
+      <c r="B171" s="19"/>
+    </row>
+    <row r="172" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="18"/>
+      <c r="B172" s="19"/>
+    </row>
+    <row r="173" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="18"/>
+      <c r="B173" s="19"/>
+    </row>
+    <row r="174" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="18"/>
+      <c r="B174" s="19"/>
+    </row>
+    <row r="175" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="18"/>
+      <c r="B175" s="19"/>
+    </row>
+    <row r="176" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="18"/>
+      <c r="B176" s="19"/>
+    </row>
+    <row r="177" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="18"/>
+      <c r="B177" s="19"/>
+    </row>
+    <row r="178" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="18"/>
+      <c r="B178" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -2834,1279 +4706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2B85B4-77BB-514B-878C-DDA4580BABC6}">
-  <dimension ref="A1:C110"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="12.5" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" ht="133" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-    </row>
-    <row r="10" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-    </row>
-    <row r="11" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-    </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-    </row>
-    <row r="13" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-    </row>
-    <row r="15" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-    </row>
-    <row r="16" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-    </row>
-    <row r="17" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-    </row>
-    <row r="18" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-    </row>
-    <row r="19" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-    </row>
-    <row r="20" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-    </row>
-    <row r="21" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-    </row>
-    <row r="22" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-    </row>
-    <row r="23" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-    </row>
-    <row r="24" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-    </row>
-    <row r="25" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-    </row>
-    <row r="26" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-    </row>
-    <row r="27" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-    </row>
-    <row r="28" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-    </row>
-    <row r="29" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-    </row>
-    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-    </row>
-    <row r="32" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-    </row>
-    <row r="33" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-    </row>
-    <row r="34" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-    </row>
-    <row r="35" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-    </row>
-    <row r="36" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-    </row>
-    <row r="37" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-    </row>
-    <row r="38" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-    </row>
-    <row r="39" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-    </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-    </row>
-    <row r="41" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-    </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-    </row>
-    <row r="43" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-    </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="45" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-    </row>
-    <row r="46" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-    </row>
-    <row r="47" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-    </row>
-    <row r="48" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-    </row>
-    <row r="49" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-    </row>
-    <row r="50" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-    </row>
-    <row r="51" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-    </row>
-    <row r="52" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="19"/>
-    </row>
-    <row r="53" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-    </row>
-    <row r="54" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-    </row>
-    <row r="55" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
-      <c r="B55" s="19"/>
-    </row>
-    <row r="56" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-    </row>
-    <row r="57" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-    </row>
-    <row r="58" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="19"/>
-    </row>
-    <row r="59" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="19"/>
-    </row>
-    <row r="60" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="19"/>
-    </row>
-    <row r="61" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="19"/>
-    </row>
-    <row r="62" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="19"/>
-    </row>
-    <row r="63" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
-      <c r="B63" s="19"/>
-    </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="19"/>
-    </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
-      <c r="B65" s="19"/>
-    </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
-      <c r="B66" s="19"/>
-    </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="19"/>
-    </row>
-    <row r="68" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
-      <c r="B68" s="19"/>
-    </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="19"/>
-    </row>
-    <row r="70" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="18"/>
-      <c r="B70" s="19"/>
-    </row>
-    <row r="71" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="18"/>
-      <c r="B71" s="19"/>
-    </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
-      <c r="B72" s="19"/>
-    </row>
-    <row r="73" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="19"/>
-    </row>
-    <row r="74" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="18"/>
-      <c r="B74" s="19"/>
-    </row>
-    <row r="75" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
-      <c r="B75" s="19"/>
-    </row>
-    <row r="76" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="18"/>
-      <c r="B76" s="19"/>
-    </row>
-    <row r="77" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
-      <c r="B77" s="19"/>
-    </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
-      <c r="B78" s="19"/>
-    </row>
-    <row r="79" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="19"/>
-    </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="19"/>
-    </row>
-    <row r="81" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="18"/>
-      <c r="B81" s="19"/>
-    </row>
-    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
-      <c r="B82" s="19"/>
-    </row>
-    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
-      <c r="B83" s="19"/>
-    </row>
-    <row r="84" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="18"/>
-      <c r="B84" s="19"/>
-    </row>
-    <row r="85" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
-      <c r="B85" s="19"/>
-    </row>
-    <row r="86" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="19"/>
-    </row>
-    <row r="87" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="18"/>
-      <c r="B87" s="19"/>
-    </row>
-    <row r="88" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19"/>
-    </row>
-    <row r="89" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
-      <c r="B89" s="19"/>
-    </row>
-    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19"/>
-    </row>
-    <row r="91" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="18"/>
-      <c r="B91" s="19"/>
-    </row>
-    <row r="92" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="18"/>
-      <c r="B92" s="19"/>
-    </row>
-    <row r="93" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19"/>
-    </row>
-    <row r="94" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="18"/>
-      <c r="B94" s="19"/>
-    </row>
-    <row r="95" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="18"/>
-      <c r="B95" s="19"/>
-    </row>
-    <row r="96" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19"/>
-    </row>
-    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19"/>
-    </row>
-    <row r="98" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19"/>
-    </row>
-    <row r="99" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="18"/>
-      <c r="B99" s="19"/>
-    </row>
-    <row r="100" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19"/>
-    </row>
-    <row r="101" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19"/>
-    </row>
-    <row r="102" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19"/>
-    </row>
-    <row r="103" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="18"/>
-      <c r="B103" s="19"/>
-    </row>
-    <row r="104" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19"/>
-    </row>
-    <row r="105" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="18"/>
-      <c r="B105" s="19"/>
-    </row>
-    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19"/>
-    </row>
-    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19"/>
-    </row>
-    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19"/>
-    </row>
-    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="18"/>
-      <c r="B109" s="19"/>
-    </row>
-    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N178"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
-    <col min="3" max="9" width="5.5" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="12.5" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="32" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="114" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>253</v>
-      </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-    </row>
-    <row r="3" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="30"/>
-    </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12" s="30"/>
-    </row>
-    <row r="13" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B13" s="15"/>
-    </row>
-    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="19"/>
-    </row>
-    <row r="15" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="19"/>
-    </row>
-    <row r="16" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29"/>
-      <c r="B16" s="19"/>
-    </row>
-    <row r="17" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-    </row>
-    <row r="18" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-    </row>
-    <row r="20" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-    </row>
-    <row r="22" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-    </row>
-    <row r="24" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-    </row>
-    <row r="25" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-    </row>
-    <row r="26" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-    </row>
-    <row r="27" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-    </row>
-    <row r="29" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-    </row>
-    <row r="31" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
-    </row>
-    <row r="32" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-    </row>
-    <row r="33" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-    </row>
-    <row r="34" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-    </row>
-    <row r="35" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
-    </row>
-    <row r="36" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-    </row>
-    <row r="37" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-    </row>
-    <row r="38" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-    </row>
-    <row r="39" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-    </row>
-    <row r="40" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15"/>
-    </row>
-    <row r="41" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-    </row>
-    <row r="42" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15"/>
-    </row>
-    <row r="43" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-    </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="45" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
-    </row>
-    <row r="46" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-    </row>
-    <row r="47" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="15"/>
-    </row>
-    <row r="48" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-    </row>
-    <row r="49" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="15"/>
-    </row>
-    <row r="50" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-    </row>
-    <row r="51" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-    </row>
-    <row r="52" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="19"/>
-    </row>
-    <row r="53" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-    </row>
-    <row r="54" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-    </row>
-    <row r="55" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="15"/>
-    </row>
-    <row r="56" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-    </row>
-    <row r="57" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-    </row>
-    <row r="58" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="15"/>
-    </row>
-    <row r="59" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="19"/>
-    </row>
-    <row r="60" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="10"/>
-      <c r="B60" s="11"/>
-    </row>
-    <row r="61" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="15"/>
-    </row>
-    <row r="62" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="19"/>
-    </row>
-    <row r="63" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
-      <c r="B63" s="19"/>
-    </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="19"/>
-    </row>
-    <row r="65" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="10"/>
-      <c r="B65" s="11"/>
-    </row>
-    <row r="66" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="19"/>
-    </row>
-    <row r="68" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="15"/>
-    </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="19"/>
-    </row>
-    <row r="70" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="10"/>
-      <c r="B70" s="11"/>
-    </row>
-    <row r="71" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="15"/>
-    </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
-      <c r="B72" s="19"/>
-    </row>
-    <row r="73" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="19"/>
-    </row>
-    <row r="74" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
-      <c r="B74" s="15"/>
-    </row>
-    <row r="75" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
-      <c r="B75" s="19"/>
-    </row>
-    <row r="76" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="15"/>
-    </row>
-    <row r="77" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
-      <c r="B77" s="19"/>
-    </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
-      <c r="B78" s="19"/>
-    </row>
-    <row r="79" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="19"/>
-    </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="19"/>
-    </row>
-    <row r="81" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="18"/>
-      <c r="B81" s="19"/>
-    </row>
-    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
-      <c r="B82" s="19"/>
-    </row>
-    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
-      <c r="B83" s="19"/>
-    </row>
-    <row r="84" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="18"/>
-      <c r="B84" s="19"/>
-    </row>
-    <row r="85" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
-      <c r="B85" s="19"/>
-    </row>
-    <row r="86" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="19"/>
-    </row>
-    <row r="87" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="18"/>
-      <c r="B87" s="19"/>
-    </row>
-    <row r="88" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19"/>
-    </row>
-    <row r="89" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
-      <c r="B89" s="19"/>
-    </row>
-    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19"/>
-    </row>
-    <row r="91" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="18"/>
-      <c r="B91" s="19"/>
-    </row>
-    <row r="92" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="18"/>
-      <c r="B92" s="19"/>
-    </row>
-    <row r="93" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19"/>
-    </row>
-    <row r="94" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="18"/>
-      <c r="B94" s="19"/>
-    </row>
-    <row r="95" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="18"/>
-      <c r="B95" s="19"/>
-    </row>
-    <row r="96" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19"/>
-    </row>
-    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19"/>
-    </row>
-    <row r="98" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19"/>
-    </row>
-    <row r="99" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="18"/>
-      <c r="B99" s="19"/>
-    </row>
-    <row r="100" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19"/>
-    </row>
-    <row r="101" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19"/>
-    </row>
-    <row r="102" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19"/>
-    </row>
-    <row r="103" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="18"/>
-      <c r="B103" s="19"/>
-    </row>
-    <row r="104" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19"/>
-    </row>
-    <row r="105" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="18"/>
-      <c r="B105" s="19"/>
-    </row>
-    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19"/>
-    </row>
-    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19"/>
-    </row>
-    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19"/>
-    </row>
-    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="18"/>
-      <c r="B109" s="19"/>
-    </row>
-    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19"/>
-    </row>
-    <row r="111" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="18"/>
-      <c r="B111" s="19"/>
-    </row>
-    <row r="112" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="18"/>
-      <c r="B112" s="19"/>
-    </row>
-    <row r="113" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="18"/>
-      <c r="B113" s="19"/>
-    </row>
-    <row r="114" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="18"/>
-      <c r="B114" s="19"/>
-    </row>
-    <row r="115" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="18"/>
-      <c r="B115" s="19"/>
-    </row>
-    <row r="116" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="18"/>
-      <c r="B116" s="19"/>
-    </row>
-    <row r="117" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="18"/>
-      <c r="B117" s="19"/>
-    </row>
-    <row r="118" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="18"/>
-      <c r="B118" s="19"/>
-    </row>
-    <row r="119" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="18"/>
-      <c r="B119" s="19"/>
-    </row>
-    <row r="120" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="18"/>
-      <c r="B120" s="19"/>
-    </row>
-    <row r="121" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="18"/>
-      <c r="B121" s="19"/>
-    </row>
-    <row r="122" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="18"/>
-      <c r="B122" s="19"/>
-    </row>
-    <row r="123" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="18"/>
-      <c r="B123" s="19"/>
-    </row>
-    <row r="124" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="18"/>
-      <c r="B124" s="19"/>
-    </row>
-    <row r="125" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="18"/>
-      <c r="B125" s="19"/>
-    </row>
-    <row r="126" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="18"/>
-      <c r="B126" s="19"/>
-    </row>
-    <row r="127" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="18"/>
-      <c r="B127" s="19"/>
-    </row>
-    <row r="128" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="18"/>
-      <c r="B128" s="19"/>
-    </row>
-    <row r="129" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="18"/>
-      <c r="B129" s="19"/>
-    </row>
-    <row r="130" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="18"/>
-      <c r="B130" s="19"/>
-    </row>
-    <row r="131" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="18"/>
-      <c r="B131" s="19"/>
-    </row>
-    <row r="132" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="18"/>
-      <c r="B132" s="19"/>
-    </row>
-    <row r="133" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="18"/>
-      <c r="B133" s="19"/>
-    </row>
-    <row r="134" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="18"/>
-      <c r="B134" s="19"/>
-    </row>
-    <row r="135" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="18"/>
-      <c r="B135" s="19"/>
-    </row>
-    <row r="136" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="18"/>
-      <c r="B136" s="19"/>
-    </row>
-    <row r="137" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="18"/>
-      <c r="B137" s="19"/>
-    </row>
-    <row r="138" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="18"/>
-      <c r="B138" s="19"/>
-    </row>
-    <row r="139" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="18"/>
-      <c r="B139" s="19"/>
-    </row>
-    <row r="140" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="18"/>
-      <c r="B140" s="19"/>
-    </row>
-    <row r="141" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="18"/>
-      <c r="B141" s="19"/>
-    </row>
-    <row r="142" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="18"/>
-      <c r="B142" s="19"/>
-    </row>
-    <row r="143" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="18"/>
-      <c r="B143" s="19"/>
-    </row>
-    <row r="144" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="18"/>
-      <c r="B144" s="19"/>
-    </row>
-    <row r="145" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="18"/>
-      <c r="B145" s="19"/>
-    </row>
-    <row r="146" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="18"/>
-      <c r="B146" s="19"/>
-    </row>
-    <row r="147" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="18"/>
-      <c r="B147" s="19"/>
-    </row>
-    <row r="148" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="18"/>
-      <c r="B148" s="19"/>
-    </row>
-    <row r="149" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="18"/>
-      <c r="B149" s="19"/>
-    </row>
-    <row r="150" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="18"/>
-      <c r="B150" s="19"/>
-    </row>
-    <row r="151" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="18"/>
-      <c r="B151" s="19"/>
-    </row>
-    <row r="152" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="18"/>
-      <c r="B152" s="19"/>
-    </row>
-    <row r="153" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="18"/>
-      <c r="B153" s="19"/>
-    </row>
-    <row r="154" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="18"/>
-      <c r="B154" s="19"/>
-    </row>
-    <row r="155" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="18"/>
-      <c r="B155" s="19"/>
-    </row>
-    <row r="156" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="18"/>
-      <c r="B156" s="19"/>
-    </row>
-    <row r="157" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="18"/>
-      <c r="B157" s="19"/>
-    </row>
-    <row r="158" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="18"/>
-      <c r="B158" s="19"/>
-    </row>
-    <row r="159" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="18"/>
-      <c r="B159" s="19"/>
-    </row>
-    <row r="160" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="18"/>
-      <c r="B160" s="19"/>
-    </row>
-    <row r="161" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="18"/>
-      <c r="B161" s="19"/>
-    </row>
-    <row r="162" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="18"/>
-      <c r="B162" s="19"/>
-    </row>
-    <row r="163" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="18"/>
-      <c r="B163" s="19"/>
-    </row>
-    <row r="164" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="18"/>
-      <c r="B164" s="19"/>
-    </row>
-    <row r="165" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="18"/>
-      <c r="B165" s="19"/>
-    </row>
-    <row r="166" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="18"/>
-      <c r="B166" s="19"/>
-    </row>
-    <row r="167" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="18"/>
-      <c r="B167" s="19"/>
-    </row>
-    <row r="168" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="18"/>
-      <c r="B168" s="19"/>
-    </row>
-    <row r="169" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="18"/>
-      <c r="B169" s="19"/>
-    </row>
-    <row r="170" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="18"/>
-      <c r="B170" s="19"/>
-    </row>
-    <row r="171" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="18"/>
-      <c r="B171" s="19"/>
-    </row>
-    <row r="172" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="18"/>
-      <c r="B172" s="19"/>
-    </row>
-    <row r="173" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="18"/>
-      <c r="B173" s="19"/>
-    </row>
-    <row r="174" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="18"/>
-      <c r="B174" s="19"/>
-    </row>
-    <row r="175" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="18"/>
-      <c r="B175" s="19"/>
-    </row>
-    <row r="176" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="18"/>
-      <c r="B176" s="19"/>
-    </row>
-    <row r="177" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="18"/>
-      <c r="B177" s="19"/>
-    </row>
-    <row r="178" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="18"/>
-      <c r="B178" s="19"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H149"/>
   <sheetViews>
@@ -5078,11 +5678,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M204"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -7186,7 +7786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F281889-6F7D-6848-B2D8-E5309E5A8CBE}">
   <dimension ref="A1:D112"/>
   <sheetViews>
@@ -7712,7 +8312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R191"/>
   <sheetViews>
@@ -10053,7 +10653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3D86EB-5946-5242-8C7B-21D23DF46C86}">
   <dimension ref="A1:F110"/>
   <sheetViews>
@@ -10684,7 +11284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456F4B46-E245-DB4D-BC75-1E1265C64598}">
   <dimension ref="A1:Z136"/>
   <sheetViews>
@@ -12402,7 +13002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J186"/>
   <sheetViews>
@@ -13971,515 +14571,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C75824-A823-0940-8E8F-EA7B7D338F3B}">
-  <dimension ref="A1:D110"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="6" customWidth="1"/>
-    <col min="3" max="4" width="5.5" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="12.5" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="67" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="D6" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-    </row>
-    <row r="10" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-    </row>
-    <row r="12" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-    </row>
-    <row r="13" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-    </row>
-    <row r="15" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-    </row>
-    <row r="16" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-    </row>
-    <row r="17" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-    </row>
-    <row r="18" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-    </row>
-    <row r="19" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-    </row>
-    <row r="20" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-    </row>
-    <row r="21" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-    </row>
-    <row r="22" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-    </row>
-    <row r="23" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-    </row>
-    <row r="24" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-    </row>
-    <row r="25" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-    </row>
-    <row r="26" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-    </row>
-    <row r="27" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-    </row>
-    <row r="28" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-    </row>
-    <row r="29" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-    </row>
-    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-    </row>
-    <row r="32" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-    </row>
-    <row r="33" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-    </row>
-    <row r="34" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-    </row>
-    <row r="35" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-    </row>
-    <row r="36" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-    </row>
-    <row r="37" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-    </row>
-    <row r="38" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-    </row>
-    <row r="39" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-    </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-    </row>
-    <row r="41" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-    </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-    </row>
-    <row r="43" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-    </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="45" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-    </row>
-    <row r="46" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-    </row>
-    <row r="47" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-    </row>
-    <row r="48" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-    </row>
-    <row r="49" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-    </row>
-    <row r="50" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-    </row>
-    <row r="51" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-    </row>
-    <row r="52" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="19"/>
-    </row>
-    <row r="53" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-    </row>
-    <row r="54" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-    </row>
-    <row r="55" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
-      <c r="B55" s="19"/>
-    </row>
-    <row r="56" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-    </row>
-    <row r="57" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-    </row>
-    <row r="58" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="19"/>
-    </row>
-    <row r="59" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="19"/>
-    </row>
-    <row r="60" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="19"/>
-    </row>
-    <row r="61" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="19"/>
-    </row>
-    <row r="62" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="19"/>
-    </row>
-    <row r="63" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
-      <c r="B63" s="19"/>
-    </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="19"/>
-    </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
-      <c r="B65" s="19"/>
-    </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
-      <c r="B66" s="19"/>
-    </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="19"/>
-    </row>
-    <row r="68" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
-      <c r="B68" s="19"/>
-    </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="19"/>
-    </row>
-    <row r="70" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="18"/>
-      <c r="B70" s="19"/>
-    </row>
-    <row r="71" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="18"/>
-      <c r="B71" s="19"/>
-    </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
-      <c r="B72" s="19"/>
-    </row>
-    <row r="73" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="19"/>
-    </row>
-    <row r="74" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="18"/>
-      <c r="B74" s="19"/>
-    </row>
-    <row r="75" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
-      <c r="B75" s="19"/>
-    </row>
-    <row r="76" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="18"/>
-      <c r="B76" s="19"/>
-    </row>
-    <row r="77" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
-      <c r="B77" s="19"/>
-    </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
-      <c r="B78" s="19"/>
-    </row>
-    <row r="79" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="19"/>
-    </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="19"/>
-    </row>
-    <row r="81" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="18"/>
-      <c r="B81" s="19"/>
-    </row>
-    <row r="82" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
-      <c r="B82" s="19"/>
-    </row>
-    <row r="83" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
-      <c r="B83" s="19"/>
-    </row>
-    <row r="84" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="18"/>
-      <c r="B84" s="19"/>
-    </row>
-    <row r="85" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
-      <c r="B85" s="19"/>
-    </row>
-    <row r="86" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="19"/>
-    </row>
-    <row r="87" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="18"/>
-      <c r="B87" s="19"/>
-    </row>
-    <row r="88" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19"/>
-    </row>
-    <row r="89" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
-      <c r="B89" s="19"/>
-    </row>
-    <row r="90" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19"/>
-    </row>
-    <row r="91" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="18"/>
-      <c r="B91" s="19"/>
-    </row>
-    <row r="92" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="18"/>
-      <c r="B92" s="19"/>
-    </row>
-    <row r="93" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19"/>
-    </row>
-    <row r="94" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="18"/>
-      <c r="B94" s="19"/>
-    </row>
-    <row r="95" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="18"/>
-      <c r="B95" s="19"/>
-    </row>
-    <row r="96" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19"/>
-    </row>
-    <row r="97" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19"/>
-    </row>
-    <row r="98" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19"/>
-    </row>
-    <row r="99" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="18"/>
-      <c r="B99" s="19"/>
-    </row>
-    <row r="100" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19"/>
-    </row>
-    <row r="101" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19"/>
-    </row>
-    <row r="102" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19"/>
-    </row>
-    <row r="103" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="18"/>
-      <c r="B103" s="19"/>
-    </row>
-    <row r="104" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19"/>
-    </row>
-    <row r="105" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="18"/>
-      <c r="B105" s="19"/>
-    </row>
-    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19"/>
-    </row>
-    <row r="107" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19"/>
-    </row>
-    <row r="108" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19"/>
-    </row>
-    <row r="109" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="18"/>
-      <c r="B109" s="19"/>
-    </row>
-    <row r="110" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100693BD51F8350324485FD573DEA5308EA" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3a5ad946f0818aa27759232261042403">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bcfd11aa4d094f7496148c95fffd8c5">
     <xsd:element name="properties">
@@ -14593,33 +14700,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2CD40-074F-4B13-A731-DCA6003B0A5A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14640,9 +14724,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2CD40-074F-4B13-A731-DCA6003B0A5A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6A85AE0-F28C-47F4-95B0-7F7590CEBA63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>